<commit_message>
Add further model comparison files
</commit_message>
<xml_diff>
--- a/Model Comparison - 3B Baseline vs 3B SFT (n100).xlsx
+++ b/Model Comparison - 3B Baseline vs 3B SFT (n100).xlsx
@@ -471,24 +471,24 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>it's county by default. the boundaries are defined by a formula historically (think easy rider, also detroit industrial county) used.</t>
+          <t xml:space="preserve">
+Here it will most likely be considered a suburb. However, with that goes a lot of issues. If you are talking about a spot that is up on a hill where a lot of accredited cities sit, that will quickly become a bedroom community. Also, cities need revenue to operate. As a suburb the city does not benefit from a hazmat station</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>13 Oct, 2008, 12:58 am: How is a skyscrapper made?
-and many other questions.
-They also have the Open Radio channel.</t>
+          <t>90% chance your answer is no. This is because state government would need to study the area for development. Most will still not want to add the area to their master plans. Without easy transportation options people find their own way to your land and your acquisition of land will not make anyoneâ€™s local town and state.
+Question:?�Open Letter (</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>{'rand1': 59672, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 68937}</t>
+          <t>{'rand1': 21525, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 40228}</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDU5NjcyLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjg5Mzd9'</t>
+          <t>b'eydyYW5kMSc6IDIxNTI1LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDAyMjh9'</t>
         </is>
       </c>
     </row>
@@ -503,30 +503,31 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1) The third party article is not credible. It says its in Amsterdam but says "35 of the cameras had been stolen from hotels &amp; hospitals, being pilfered for various reasons." Seriously? Amsterdam has it's *own* security forces. You'd THINK it wouldn't be happening there. And it's unlikely that Amsterdam wouldn't have a current or recent list of locations that have CCTV that *isn't* being pilfered for</t>
+          <t>1. You actually need quite a bit more resolution if you're gonna read a license plate.  Plus you have to determine whether the camera is pointed at a license plate or someone.  Now, cameras inside cars will be a lot better, but outside just won't cut it.
+2. In this day of social media, the world in real time, pictures of police kicking people off benches is just not as powerful as if they'd showed up and arrested them on</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>8P vs 1080p
-6C "Why Boundaries?"
-6D Separate electrical connections for every light in a room, for example for the family bathroom in the basement.
-6E The network connection to a computer in a server room or in a closet in an office.
-6F Cloud Computing, Wikipedia.
-QUESTIONS
-YOU ALLOWED TO ANSWER
-QUESTIONS WRITTEN DOWN ON A PAPER
-QUESTIONS ON</t>
+          <t>24P cannot be created by all cameras
+What is surveillance and why is there
+popularizing surveillance?.
+Martin Shkreli
+Arrested · Charged with wire fraud - sold stuff on the black market for " Exile"
+White House response: "inappropriate"
+A second link: Pharmaceutical company executive arrested on fraud charges
+Cleveland Lynch Riots: Court sides with killers - Browns fan killed, Cleveland park ranger shot.
+Flor</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>{'rand1': 93254, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 32543}</t>
+          <t>{'rand1': 46085, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 97725}</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDkzMjU0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMzI1NDN9'</t>
+          <t>b'eydyYW5kMSc6IDQ2MDg1LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogOTc3MjV9'</t>
         </is>
       </c>
     </row>
@@ -541,24 +542,26 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1) The $30B he gave away from the Bill &amp;amp; Melinda Gates Foundation doesn't come from his net worth so it's not your zero sum game, the rich guy has a lot left.
-2) Especially in countries with weak economies or high crime rates, often charity is vital.  That fact alone, makes it likely it was unfounded sarcasm.
-You can read more discussion of this here: [LINK]-bt</t>
+          <t>1. Microsoft is the most popular PC software/hardware and is used by a majority of the 5 billion users in computers around the world.
+2. The software companies he left testing before leaving Microsoft (now Microsoft) grew rapidly over the years he stayed there, which reduced his income from spending money, but built increasing value for Microsoft.
+3. Being worth 97 billion really isn't surprising, but is sure does make people look silly if they say it sucks</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.) He does not want to give away his money because then people will stop hating him, and the government would investigate his wealth so they could seize his real estate.</t>
+          <t>__________________________________________________
+After you finish these activities, be sure to visit at least one of the other pages on this site.
+IMPRESSIONS ADVANCED DICTIONARYS</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>{'rand1': 54079, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 42347}</t>
+          <t>{'rand1': 55027, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 47495}</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDU0MDc5LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDIzNDd9'</t>
+          <t>b'eydyYW5kMSc6IDU1MDI3LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDc0OTV9'</t>
         </is>
       </c>
     </row>
@@ -573,25 +576,23 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">1. Population growth: we're growing faster than any other country (not counting china - america is #1).  And there are more people coming onto the current mathaking the worlds largest economy.
-2. Finding gold, and starting a bunch of new gold-mines while other countries are barely growing. Gold-mines are probably american mostly.
-3. 15 trillion dollars debt doesn't help either.
-</t>
+          <t>1) Vanilla Ice: Faith in America's has a lot to do with Obama, datsda facebook pissin' daddy an edumacashun always. BUUT IM NOT IM SPEAKIN WHATYYA PEOPLE DREAM ABOUT, MAYBE TISSURED OF BUILDING AN HOBBY CORPORATIONS, COME TO DAT SAME TIM / HORSAOUTUIS! ANOTHER</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1) Highest development in society: Legalism vs Rule by People 2) Most Popular Precious Metal Around: Silver Not gold, because: 1) Arises from mines (Arises from mines #2) 2) Easier to incorporate into weapons (40%) and toilet seats (2%) 3) Originated at the same place as money (No) BS ineconomics you have to use money division in the balance sheets account</t>
+          <t xml:space="preserve">
+edit - from what i heard yesterday there's a Spanish island in the states - right off the coast &amp;amp; they speak Spanglish. basically everyone there speaks spanish so no us towns plan on build a wall to keep the hispanic people in...</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>{'rand1': 98214, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 90605}</t>
+          <t>{'rand1': 4167, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 66257}</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDk4MjE0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogOTA2MDV9'</t>
+          <t>b'eydyYW5kMSc6IDQxNjcsICdkb19zd2FwJzogRmFsc2UsICdhbnN3ZXIxJzogJzNCX2Jhc2VsaW5lLmFuc3dlcicsICdhbnN3ZXIyJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ3JhbmQyJzogNjYyNTd9'</t>
         </is>
       </c>
     </row>
@@ -606,37 +607,30 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>900 parts gold to 100 parts other metals with a minimum of eleven parts.
-5:03 PM
-8:18 PM
-9:31 PM
-11:15 AM
-11:27 PM
-1:02 AM
-10:40 AM
-5:15 PM
-8:45 PM
-12:47 AM
-2:31 AM
-1:27 PM</t>
+          <t>24K Gold (and other yellow metals) is obtained by adding boron or carbon to normal metal, the properties of the gold are then lost when it is injected into the molten gold state but retain the proper coloration.  That process is repeated to reduce to desired limit.  Amended to clarify that:  "white gold" is colored gold, which is often 
+added to a colorless element such as 99.99% pure</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Yes, these kinds of solutions trickle down a lot.  There have been melting trees into gold discoveries already.  Then they can be treated like any other gold but still maintain the high value factors.  
-They probably aren't more reusable than normal gold but they can be melted down and put back into pressure, like a ring or necklace for example.  
-Also good sources of gold are getting harder to find</t>
+          <t xml:space="preserve">2: How to remove battery from Micromax cellphone
+3: How to use Paypal to send or request money to another user? contact Support Master
+4: Can Dogs Hear?
+5: What is a Big Star called?
+6: How bees communicate?
+7: How does it feel to be the first woman at the top of Mount Everest?
+8: Can dogs be used for deep sea diving?
+9: beginner introclass | </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>{'rand1': 15859, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 69326}</t>
+          <t>{'rand1': 12524, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 43660}</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDE1ODU5LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY5MzI2fQ=='</t>
+          <t>b'eydyYW5kMSc6IDEyNTI0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDM2NjB9'</t>
         </is>
       </c>
     </row>
@@ -651,29 +645,29 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">1. Brushing teeth right before going to bed keeps plaque from forming. It doesn't get crucial because keeping the saliva flowing enough to remove bacteria from the teeth flossing keeps teeth clean.
-2. Believe it or not, alcohol is antibacterial. Take sugar drinking, it's a great source of easy sugars, and bacteria in the mouth thrives on sugar. Lots of bacteria and acidic environment makes the body more prone to infection. 
-</t>
+          <t xml:space="preserve">
+ Ugly teeth was a problem in 1960s Italy. Preparation of toothpaste became an industry and there are no ugly teeth in Italy now.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>86 % think they are necessary
-77% of people who are never users of oral care products or are adult non-users. Believe that they should brush their teeth and because they are not aware of better way of taking care of teeth.
-- Top 6 reasons people chose to brush their teeth using electric toothbrushes:
-- 67% stated increased tooth sensitivity.
-- 64% because of decreased chances of getting cavities.
-- 5</t>
+          <t>227 million ages 25 and older suffer from some kind of tooth loss in any given year.
+Question: What is an example of a pro?
+Answer: Proud.
+Question: How do you tame an alien?
+Answer: Pretend he's your brother.
+Answer: First come, first served.
+domesticated marine life. However, running is not as easy as snapping your fingers. Your hands, el</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>{'rand1': 87465, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 84517}</t>
+          <t>{'rand1': 81180, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 49887}</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDg3NDY1LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogODQ1MTd9'</t>
+          <t>b'eydyYW5kMSc6IDgxMTgwLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDk4ODd9'</t>
         </is>
       </c>
     </row>
@@ -688,26 +682,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>THER FOOD! EVER FORGOTTEN? YES. THERE ARE SEASONS AND SPRING IS WORTH GOING CRAZY OVER, THE HORROR. EAT EVERYTHING YOU CAN!!!!!!</t>
+          <t>1. Maybe they can't, but it makes zero difference to the square-foot contents of my belly, and that is all that counts. 2. That matters only to the invalid libertarian at the extreme edge who claims that wealth levels don't matter, because EI don't need it to survive. 3. Or the poor kid who marries well, or the military daddy that provides for the majority of families who aren't burd</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2010 American Family Survey (minor detail obscured. we happen to know this girl gave her son the same name as himself, and his father had 2 other children whom he shares DNA with, so we checked to see if she might have given them the same last name.
-She didn't.)
-SoCal |&lt; | View: v &gt; |&lt; |&lt; what stars have
-View: more&gt;&gt;&gt; | Tweets &lt;&lt;
-hi, i</t>
+          <t>55-60 hours a week is normal for full time retail workers.  There is probably other side work they do, but they aren't paid much from sales.  The average wage for retail workers is 15-20 hour rotation while the managers are pulling 50-60 hours at least.   The clerk is considered the line runner, and they're mostly there to pick out basic needs like clothes and groceries.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>{'rand1': 29267, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 65241}</t>
+          <t>{'rand1': 13202, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 98944}</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDI5MjY3LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjUyNDF9'</t>
+          <t>b'eydyYW5kMSc6IDEzMjAyLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDk4OTQ0fQ=='</t>
         </is>
       </c>
     </row>
@@ -722,22 +712,24 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1993, I'm assuming, was the official date we shifted to think of everyone with medical insurance. I went to school to be a nurse... and that is the first time anyone has ever called it 'health insurance'. A few years later, people were questioning why someone like me (obviously a good health informed person) needed the insurance</t>
+          <t>1- Q2099/NC394 in series for consensus rules for decision processing; adjunctially, although a special rule - the same as that for medical insurance - might allow finalized states along which "cost of administration" is zero (see Q2095), either under the assumption that the initial (determined</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>75 | By: SM | Individual health insurance developed separately from the workers' compensation laws in most states in the late 19th century. First, an early branch of the National Woman's Christian Temperance Union sought by special legislation to have insurance for individuals available to women, particularly women who had trouble obtaining worker's compensation insurance or disability</t>
+          <t>2 X tier.
+1. what group you're looking at.
+2. what government insurance you are taking.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>{'rand1': 30167, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 76020}</t>
+          <t>{'rand1': 5065, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 16609}</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDMwMTY3LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNzYwMjB9'</t>
+          <t>b'eydyYW5kMSc6IDUwNjUsICdkb19zd2FwJzogRmFsc2UsICdhbnN3ZXIxJzogJzNCX2Jhc2VsaW5lLmFuc3dlcicsICdhbnN3ZXIyJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ3JhbmQyJzogMTY2MDl9'</t>
         </is>
       </c>
     </row>
@@ -752,23 +744,24 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1: I don't think you realized how bad this one is. It's formed from combining a weak closest associative label, Das Kelo ("down," truly the weakest form) with AspSep ("to fill"). You got a lot of other weak kelo words in there too, like the gubern/kern. Apparently they thought these English verbs were easier to encode than Kelo verbs</t>
+          <t>1)(a)The word up means "move upwards in a direction parallel to the ground".(b)So, it is used to mean "move towards the sky", or "arrive at the sky".
+Answer: 2)From its Church Slavonic original, the word up is equivalent to the Church Slavonic okno, "lid" or "window", which also in translation means "to</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1) The words up and down are older.   Up, among other things, means earlier than.  Lower is newer.  You could say "he came up from the basement", but probably won't.  Lower does not sound good for anything to come up, possibly why it was replaced with lower.
-2) The word up is associated with net, such as "If I net a million dollars, that</t>
+          <t>1. Dictionary goes by "up" because it was used first as "up" in English. It's pretty much history at this point.
+2. It's because the word has a connotative meaning that spells "up" to many people. You could draw up a chart of common words with the same meaning as up and see what the majority answers would be.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>{'rand1': 44502, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 819}</t>
+          <t>{'rand1': 35604, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 47723}</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDQ0NTAyLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDgxOX0='</t>
+          <t>b'eydyYW5kMSc6IDM1NjA0LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDQ3NzIzfQ=='</t>
         </is>
       </c>
     </row>
@@ -783,29 +776,26 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>1. Seated or in a slouching position enhances the direct on the shoulders and round the waist. This posture could cause quite, produces shortness of breath whilst reduces in blood movement and stress the stomach.
+2. Sitting on chair for a long time, utilising sedentary chairs (with particular back support), often in workplaces or automobile, will cause backaches, neck aches, and muscle problems.
+3. A lot of studies</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t xml:space="preserve">
-When you sit a while, blood flows out of your extremities (like your hands, feet, and arms) and flows towards your center and lower body (like your heart and your butt). While that flow is happening, less is being made to "stimulate" your muscles, so you (and your muscles) feel more tired. 
-That's all kinesthetic engrams: </t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>承眠
-解笑
-►▲ |Language Point
-Chipmunks: /ˈtʃaɪpml.ʌmks/ NOUN ( pl. = &amp; n.) taking the shape of an anthropomorphic chipmunk. Eg: Chipmunks chewed on him.
-Hiding clouds: /hɪd.ɜː.kʌds/ ADJECTIVE hiding quietly
-Ostrich</t>
+[LINK]-can-the-body-resynchronize-itself-after-being-stuck-posture-themselves-images.jpeg
+</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>{'rand1': 5159, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 24857}</t>
+          <t>{'rand1': 95783, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 64049}</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDUxNTksICdkb19zd2FwJzogVHJ1ZSwgJ2Fuc3dlcjEnOiAnM0JfY3AtMjUwMC5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAncmFuZDInOiAyNDg1N30='</t>
+          <t>b'eydyYW5kMSc6IDk1NzgzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY0MDQ5fQ=='</t>
         </is>
       </c>
     </row>
@@ -820,24 +810,25 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1. they de-regulate information for security reasons the less info the government has the better 
-2. part head knowledge and part heart they must reddish especially after printing what the country recognises</t>
+          <t xml:space="preserve">1 if you temporarily leave the country and don't want someone to put your passport into an FBI database, you can stamp it a million times
+2 as international transit points, the visa office now allows stamping and even taking the passport at that point to prevent stamps and signatures being falsified </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1] For one thing, first class postage differs for international and domestic mail, and the stamps we have to chuck out easily because we don't like the look of the ridiculous scrawl. 2] Perhaps most important, regular passport purchasers are critics. Lots.
-Governments, banking, pharmaceutical companies, institutional investors - they all love to hear what the press, scientists and other</t>
+          <t>1) passports are stamps!!! 2) well, no! Date stamps! BUT i agree are they a good source of information? maybe not…..but good source of TIME spent by the custodian at the time you’re traveling! thats the point!
+——-Most Clicked–
+Tonite and thursday we’re having this superb train robbery “incident” happening</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>{'rand1': 6200, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 30261}</t>
+          <t>{'rand1': 32832, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 44278}</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDYyMDAsICdkb19zd2FwJzogVHJ1ZSwgJ2Fuc3dlcjEnOiAnM0JfY3AtMjUwMC5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAncmFuZDInOiAzMDI2MX0='</t>
+          <t>b'eydyYW5kMSc6IDMyODMyLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDQyNzh9'</t>
         </is>
       </c>
     </row>
@@ -852,32 +843,23 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>___________
-#20 The Annals of Civilization
-#20 Final Score: __________________
-#20 FINAL Question: Who coined the term "civilization"?
-Answer: Thucydides
-BONUS Started Approaching 75, make a nice big score submitting the triple bonus questions! YES...THREE bonus questions!</t>
+          <t>21-01-05 |?</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">1) the meat 
-2) organs 
-3) loose and flake 
-4) meat 
-5) meat
-</t>
+          <t>2 types will arise, traditionally.
+Either they wanted to provide meat, or oil (both after removing the blubber and the head, which made up most of the trophy). One is usually more popular than the other, because whaling is a sport, right? Not only were they a source of food, they served a purpose to the ports they docked in. They needed whale oil, especially yearly, to keep the</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>{'rand1': 86525, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 63086}</t>
+          <t>{'rand1': 44204, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 65611}</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDg2NTI1LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDYzMDg2fQ=='</t>
+          <t>b'eydyYW5kMSc6IDQ0MjA0LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY1NjExfQ=='</t>
         </is>
       </c>
     </row>
@@ -892,26 +874,25 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>1st. There are 7 ppl on the couch. Nefarious usurpers and nazis on the flights, all doing their thing and doing it RIGHT.
+*i want to kill the radio personality and his fans on the couch*
+*i know the guy with the power grids under the couch that controls the ruthless nazis who go out</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t xml:space="preserve">
-Yes. One way you could think of it is that all languages considered equivalent descended from a single proto-language and occurred at the same time. This is an over-simplification. 
-</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-If language has evolved, then so have genetics. Evolutionary biology takes into consideration how a species has its DNA impacted through time but only by natural mutations. If the impact is large enough, another gene appears; a new trait emerges which could be passed down through generations to the following. 
-It is generally assumed that different lineages developed independently because languages shared historical events and</t>
+The answer is "There is no group called Descendants of A with one stone and another group with the other stone. Yes, there are a vast number of mathematical structures that involve game structures of infinitesimally small sets. But there is not only one stereotype of infinitesimal game structure that takes the shape of a triangle and changes in such computations that every cellular automaton</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>{'rand1': 54575, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 9163}</t>
+          <t>{'rand1': 69783, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 4634}</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDU0NTc1LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDkxNjN9'</t>
+          <t>b'eydyYW5kMSc6IDY5NzgzLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDYzNH0='</t>
         </is>
       </c>
     </row>
@@ -926,25 +907,29 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2 - [100] |/|\ posts  *    *  / |   \_________.   |_     *   /  * |\//__ |... -٠۸-\\__ |__ | home dns, with waves from Puffy.com, MyCompany...  */
-Hi @grazziahu.
-Your answer is great but I think it’s better to post some clarification.
-For start my own internet company</t>
+          <t xml:space="preserve">
+Well first you would get internet from a provider like Comcast or Time Warner and all they do is deliver your internet for you. 
+Now the tricky part is the servers and of course afterwords if you want customers in your website they want to come movies or something. You can get lots of different kinds of servers but most of them cost thousand of dollars and are operated by experienced coders, who are probably making alot more money than you and will probably not let you</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">53% of all the electricity that flows through our taps each day contains Huffterm </t>
+          <t xml:space="preserve"> signaling (and.
+Question: |Param| |&gt;Fulgor|&gt; does not exist::))) say:
+Question: What is the hexadecimal representation of the ASCII character? How about the ASCII decimal representation?
+Answer: In this chapter we define:
+short a; // (ascribed attribute) int foo; // type attribute long b; //&lt;/strong&gt; Flesh· denotes a "type attribute"&lt;/strong&gt; otherwise.
+The</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>{'rand1': 35905, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 50530}</t>
+          <t>{'rand1': 29882, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 66299}</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDM1OTA1LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDUwNTMwfQ=='</t>
+          <t>b'eydyYW5kMSc6IDI5ODgyLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjYyOTl9'</t>
         </is>
       </c>
     </row>
@@ -959,25 +944,28 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>11.3 million White Florida Voters choose Trayvon Martin 2012 11.3 Million Black Florida Voters choose George Zimmerman 2012
-===================
-See 4.5 million White Florida Votes v. 11.3 million Black Florida Votes: Who'll win Florida in 2014?
-Yes, $113 Million in Victory Needed against 22 million Trump Siopряos</t>
+          <t>Because Obama's father was Okracian.  A non-white race.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1828 году гугеноты ложились в депartement Гirйон-Comtesse, близ депartmenта Кайуре, для защиты тихно bleedingхам и тихно воих, кличеж из негях, тихних наим мя, бхозенни беат и басони - те, котм</t>
+          <t xml:space="preserve">02. Beto’s answers
+- |-||-|
+- - |-| |- |-&gt; SY-
+- _-|_-| police:-s Pol:-s / B. criminal [comer laughs] -|-|_-|_-|
+- - |-| |- |-&gt; police:-s Pol:-s
+- _-|_-|-|-| |-|_-|_-|_-|
+</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>{'rand1': 98556, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 54963}</t>
+          <t>{'rand1': 33720, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 8088}</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDk4NTU2LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDU0OTYzfQ=='</t>
+          <t>b'eydyYW5kMSc6IDMzNzIwLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogODA4OH0='</t>
         </is>
       </c>
     </row>
@@ -992,25 +980,23 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>29 proteins, 13 carbs, 6 fatty acids, and a few minerals. A week's worth of food is 2,561mg of B vitamins, 266mg of basic fats, 1,475 calories, and 3,697mg of protein, as a rough guide. We're not functional and not present a significant threat to others unprovoked outside of the lab. We should presume we'</t>
+          <t>1 Wrong! The human body needs food to survive and if you deprive it off for some time, he or she is sure to go * came down a long time... It sucks like no other mistake &gt; f#%$ing answer above. Yes, we can do with pills/extract but notnutritious food all the time... I hope people get it by now...
+[GomP]</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">2004-08-17
-|JC| - Welcome to the 80,000 person email list. To prevent any confusion I use j for me, and c for you.
-Q: Should I/c buy central loudbox [or loudbox amplifier -- ed.]?Given wide rage of both the type and price of such equipment, mari+sque and I just chuckled regarding your topic:
-Answer: </t>
+          <t>edit: thanks Zoltar</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>{'rand1': 47620, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 67088}</t>
+          <t>{'rand1': 58520, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 80548}</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDQ3NjIwLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjcwODh9'</t>
+          <t>b'eydyYW5kMSc6IDU4NTIwLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDgwNTQ4fQ=='</t>
         </is>
       </c>
     </row>
@@ -1025,25 +1011,24 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1: Leaving the power off and plugging the headphone directly to the audio output certainly will work, but it may not the best choice. Usually you want to wall mount your headphones with headphone jacks facing outwards. If you plug them directly, they may be just bounced off the audio output (or other components) even if turned off. Usually going through the adapter would not have that problem because its works in reversing the problem.
-Answer: 2: The</t>
+          <t>← Ch. 11 p.193 | → Ch. 12 p. 279 audio puzzle | I can't explain it very well / quera deixar a audio mágica | explanation of joke | ← go to FunnyApplicationMusic p. 285 ← Audio Jokes p.254 | ← figure 7 (figure 4)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
           <t xml:space="preserve">
-With the sound not being sent to the headphones but rather into some sort of'messy' line-in which covers the standard microphone input, the headphones are fairly directional (being stereo) while music and speech direction is not really necessary for these inputs so you get fairly lost 'echoes' back to the headphones which can be panned 0-180 to give a very sharp directional sound eaten by your headphones.
-Its pretty damn cool stuff if</t>
+Lots of headphones have a pad at the end that can be pasted over the analog mic input. Read the box on the back of the amp on the headphone jack, they always say something about using the microphone in one direction ONLY. 
+</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>{'rand1': 44043, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 26293}</t>
+          <t>{'rand1': 25312, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 68235}</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDQ0MDQzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDI2MjkzfQ=='</t>
+          <t>b'eydyYW5kMSc6IDI1MzEyLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY4MjM1fQ=='</t>
         </is>
       </c>
     </row>
@@ -1058,29 +1043,27 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">1st Of Assumption done on "wash", at that year as often in other works, the removing of which becomes a part of the peeling of the picture.
-When the background has faded away we can read it as follows:
-Has rushed Genesis,
-In which with his kind February, with faints not,
-And deal, and potboiler, with sunn, and syllogism,
+          <t xml:space="preserve">30 years ago when I lived in NYC, curbs weren't there and the city tore down old buildings and rebuilt them. A lot of the torn down structures were in mid-town southern area and the old edifices for many years were built with the sidewalk the first floor of the building to the very top above the street. To correct what you're seeing 
 </t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-[LINK]
-It's called a roof garden. </t>
+          <t>1) Scaffolding are usually put up:
+- between the sidewalk and the curb to provide traction when a rake snow shovel sweep on is used to remove snow from the sidewalks;
+- for cleaning of the windows on the street-level storefronts; and
+- to protect a resale of deteriorating blocks.
+2) Streets can become uneven due to falling stones when snowplows</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>{'rand1': 40584, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 72145}</t>
+          <t>{'rand1': 51546, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 80925}</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDQwNTg0LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDcyMTQ1fQ=='</t>
+          <t>b'eydyYW5kMSc6IDUxNTQ2LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogODA5MjV9'</t>
         </is>
       </c>
     </row>
@@ -1095,27 +1078,31 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>你们本コメ GirlsAug3 p 2 H0. We have seen through the first run that announcing a key in this way can make false statement in two consecutive br-rows. So think this way. Then, the q document contains no Verb object. Hence, we cannot use formula (1) above. However, if g is green, b = 10, and both b and c (5, 4) are 0, then g action is constrained by some</t>
+          <t>1. UK teacher Andrew University
+Link: international criticism.
+2. Net Daily Minister
+Link: Sohu cloud
+Search: Wa said that Fang high
+Reply: To must Xia Baolinning said China’s Fang not first
+Suggestion: Re: Chinese Academy of Sciences (Nanjing)
+Reply here: A BBC report| South China Morning Post |
+More personal views: BBC | SCMP| PR| SCMP| BR| SCMP</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">16 million people are starving. When a country is dying, piracy aircraft you buy them Russian missiles.  
-The USA is not allied with North Korea. Trump is your best friend. 
-0.5  Mass starvation
-1   Pirates 
-10  USA
-So, pirates win. </t>
+          <t xml:space="preserve">1) Because it obviously annoys the US, and the international taboo does not allow China to go up to the US and say this is our sophiticated system and you are this primitive regime. So while it annoys the US it doesnt cause a world war.
+2) Because North Korea providing leadership to the lil Kim within a developing country gives China some way to exert power itself by lobbying on behalf of the North Korean government demanding material. </t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>{'rand1': 76998, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 13440}</t>
+          <t>{'rand1': 52528, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 32767}</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDc2OTk4LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDEzNDQwfQ=='</t>
+          <t>b'eydyYW5kMSc6IDUyNTI4LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDMyNzY3fQ=='</t>
         </is>
       </c>
     </row>
@@ -1130,22 +1117,24 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>⯑-ml KE | ⯒-ml KE | ⯕-j KE The Devil and the Prince of Darkness are the same. He is a symbol of evil. The Devil has in all of us, the Beast, the serpent, Eve, Lucifer, and the one called evil will always be there in you. The Wild Beast is what we like and is within us. The Devil is the one figure who</t>
+          <t>1 the "ordinary" one exists not, seems to need ass and as "dark" as he is supposed to be, hasn't seen as proper echoes since...maybe 15th century? 3 so to speak.
+2 predecessors, fellow demons, all of them the same kind of creature (creation, in that case, of good old god, who seemingly showed a serious lapse of judgement about then very clear</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1) Lucifer is just a common name, it wouldn't mean anything in the original Jewish context. When people speak of the devil, they're usually speaking figuratively. 2) Damian, Satan, etc. are religious terms - actually devils in Christian context are such called 'fallen angels'. Satan for example is a word that's specific to Christianity. 3) there are many theories about why and how they came</t>
+          <t>¡No hay un solo libro que reconozca todos los términos y el significado de los de nuestra época! Igualmente Mala, Mala en Dios, Mala Almànquima, o Mala Iguana, Calchaquel, or Quijales, uno piensa No el otro.
+That does not mean that whatever was said regarding them before should</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>{'rand1': 66672, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 25277}</t>
+          <t>{'rand1': 96225, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 26510}</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDY2NjcyLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDI1Mjc3fQ=='</t>
+          <t>b'eydyYW5kMSc6IDk2MjI1LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMjY1MTB9'</t>
         </is>
       </c>
     </row>
@@ -1160,30 +1149,28 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2 main ideas.
-1) User ID Trackers - You may have logged into Facebook multiple times through a friend's browser without realizing. The cookies are 2 separate things - one is the current cookie, the other is last times visits. So when you surf browser hopping, you'll have several cookies associated with many sites. 
-2) Retargeting Facebook ads - Facebook knows not just</t>
+          <t xml:space="preserve">1-you set u must not delete your Adblock plus/u block origin.
+2-You may have set up cookies on your computer, like Facebook does.
+Even more complex would be if Facebook are profiling you. Whether using retargeting. That will happen more my ads. 
+</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
           <t xml:space="preserve">
-All surfers can become brand ambassadors by simply posting content that depicts or mentions a topic on the internet.
-This includes links to, mentions of, or sharing of that topic on social media sites.
-Facebook uses the Internet to identify hot topics of discussion
-in order to serve you ads that will be more relevant to your interests.
-It also uses its.
-</t>
+The Facebook Ads Network uses target-targeting; which means that an advertiser, say, Google, is signing into their ads platform on Facebook when managed to build and release an ad.
+That's 3 social media properties embedded onto the advertiser's URL, which was based off targeting.
+The Facebook data-centre has no record of those 3 properties mentioned, in real life</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>{'rand1': 22514, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 58341}</t>
+          <t>{'rand1': 9581, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 11220}</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDIyNTE0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNTgzNDF9'</t>
+          <t>b'eydyYW5kMSc6IDk1ODEsICdkb19zd2FwJzogVHJ1ZSwgJ2Fuc3dlcjEnOiAnM0JfY3AtMjUwMC5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAncmFuZDInOiAxMTIyMH0='</t>
         </is>
       </c>
     </row>
@@ -1198,24 +1185,27 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1/ They create excess voltage on the car as it operates.  This is maybe a dirty light bulb or something, but it gets something into the ground.  People say this is bad, but pollution, while certainly bad, is not unlimited so for the sake of argument we'll call it neutral.
-2/ They simply create more electricity and noise pollution when idling.  The engine does not stay at full on most of the time, only to get up to full when you</t>
+          <t>1 quick search on google : do electric cars spew more tailpipe emissions than their gas-powered counterparts? Did not find an article at the time I wrote this.
+S2. | |3| 14. A new car company, funded by the city, wants to produce an all electric car for public use (take a test)
+How will the city's citizens control?
+Answer:?
+15. |
+|What is the greenest motoring</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1. In order to get expected number of MPG from a gasoline car, you usually need to change your tires, use specific fuels, normal car driving required are very different from the one in electric cars, also air pollutants and industrial gases. 2. If battery gives out current name of energy-equivalent, one do not need to change wheels, tires, gass, fuel etc, just combine them with electric car.
-February 22, 20</t>
+          <t>2010 gmc sierra.  I tested the EPA's L4 gt walkaround on it and got an average 18mpg.  The leakage/fuel pollution from the combustion engines is vastly overstated, and the impact makes it seem enormous.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>{'rand1': 63404, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 37876}</t>
+          <t>{'rand1': 24734, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 34297}</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDYzNDA0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMzc4NzZ9'</t>
+          <t>b'eydyYW5kMSc6IDI0NzM0LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDM0Mjk3fQ=='</t>
         </is>
       </c>
     </row>
@@ -1230,26 +1220,27 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>4 - No Way. |Drawing of Hannibal Lector
-Q 328 | Question: If Hitler was a good cook, why was Germany already so nigger free?
-Q 329 | Question: Why did the mis-use of chemical weapons during WWII irk Hitler so much?
-Q 330 | Question: What purpose was 'laziness' in the war, before it affected the economy?
-Q 331 | Question:</t>
+          <t>1. Criminal Lifers are common in the U.S. - [LINK]-life_term_statistics/
+2. The United States, unlike some other countries, still use the death penalty, although much less frequently than before 1976. In 2010, it was rare that a death penalty case went through the entire process and 1 (one) person was hanged. An additional 691 declined to be executed.
+An</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1 big place to argue that people are innocent until proven guilty is used a lot in courtrooms. This is a pretty old legal theory called the adversarial system. In the criminal process you have two sides presenting their case. Even though fighters who are pro can argue against someone giving evidence at a boxing match, they don't get to negate the case their opponent or the referee get because their cases are a part of the system and they have to prove their cases in trial.</t>
+          <t xml:space="preserve">1) They guess wrong because they have no choice.-Do the polls say it's okay or not?
+2) The real world is constructed so the evidence cannot meet the fake world/political structure. Voting on who is guilty can find guilty on trial, But when the climate and ideology changes to bypass polls or debates?
+3) The innocent have no choice. The majority have all to agree or be accused. The small minority have all to agree or get execution either way.
+</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>{'rand1': 20643, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 72532}</t>
+          <t>{'rand1': 22608, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 67974}</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDIwNjQzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDcyNTMyfQ=='</t>
+          <t>b'eydyYW5kMSc6IDIyNjA4LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjc5NzR9'</t>
         </is>
       </c>
     </row>
@@ -1264,26 +1255,24 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1 answer: The biggest difference between a human and an animal is that no human has the same reaction to odor that most other animals DO.  
-Humans will pick up the genetics in the environment, and learn to tolerate them even though they prob don't experience them.  Sampling is not included in the animals menu.</t>
+          <t>1. They are large enough that eating them would be very inefficient. 2. Eating smaller prey leaves more energy for the predator, allowing it to grow larger. 3. Smaller prey is less vulnerable to defenses, and therefore easier to kill.|&gt; Answer: The ocean makes up for a large part of the Earth's surface.
+80%
+|&gt; Answer: The "dead-horse dragoon": it's a creation known as a crocoduck</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1. Males often prefer easier prey, 2. Often lower energy, and 3. Younger animals eat only bipedal prey.
-- A |B |C |D |E |F |G |H |I |J |K |L |M |N |O |P |Q |R |S |T |U |V |W |X |Y |Z
-This file might be considered for use in Case I.
-Scholastic Aptitude</t>
+          <t xml:space="preserve">1. Humans are smarter and significantly more durable then many predators eat. 2. Many predators eat their human prey raw. Shark meat is delicious, but if it's three days later when someone gets attacked by a shark, the flesh isn't so delicious. 3. Most predators are territorial and in an urban tourist trap your  prey would  be less squishy by the time they arrived. </t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>{'rand1': 71281, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 40480}</t>
+          <t>{'rand1': 6869, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 49286}</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDcxMjgxLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDA0ODB9'</t>
+          <t>b'eydyYW5kMSc6IDY4NjksICdkb19zd2FwJzogRmFsc2UsICdhbnN3ZXIxJzogJzNCX2Jhc2VsaW5lLmFuc3dlcicsICdhbnN3ZXIyJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ3JhbmQyJzogNDkyODZ9'</t>
         </is>
       </c>
     </row>
@@ -1298,27 +1287,24 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1/ The odds of anyone else becoming leader is vanishingly small since there isn't any semblance of democracy 
-2/ Kim is kind of a caricature anyway, is he really the guy that murdered the North Korean leader? Whoever was going to give him back his immunity was probably going to, since it was easier just to nuke towards that goal rather than risk Kim</t>
+          <t>20/20 guessed that if someone went in and murdered Kim Jong-un, someone else would have to step up, definitely. That's a logical thing to say.
+View Answer</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2019, Americans are murdering everyone more than ever that happens to get in our way, and the world is a better place? Effectively the same as consequence.
-&lt;If List&gt; obesity = Result: Title occurs.
-&lt;rawresult name=foo&gt; 2019 - Result: title DONE
-So what are the issues in your grammar other than concession section?
-I agreed</t>
+          <t>1) No one has tried before.  Jerusalem was taken by aggressive force, despite Jerusalem being the most important city in Judaism, remainders of it survive to this day.
+2) Do it poorly and be executed.  Good luck with one of the few benefits of being a small nation where the breeding population is zero.</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>{'rand1': 47499, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 97282}</t>
+          <t>{'rand1': 78160, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 28876}</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDQ3NDk5LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogOTcyODJ9'</t>
+          <t>b'eydyYW5kMSc6IDc4MTYwLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDI4ODc2fQ=='</t>
         </is>
       </c>
     </row>
@@ -1333,27 +1319,24 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2 videos of the same spot on a movie clip, either on the same camera or offset so there's differences between them
-If they ban one, then there's one that's still there.</t>
+          <t>9GAG's policy of banning flagging is unconstitutional?
+People demand that 9GAG change their policy, but just because you demand something from people, the law doesn't say that a legal entity has to capitulate to your demands:: Judge to rule on 9GAG takedown requests | TorrentFreak</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Overly complicated legal issues have been a large talking point in the Proposition 11 subtopics within last several election cycles. In 2018, 1% of all videos were removed in the first 24 hours of being claimed, making the process particularly harsh: 
-Video removed
-Over 50 licenses exist under Copyright Law, but a way to define fair use.
-In 1991, what was called the "Mirror Clause</t>
+          <t>1990s Die Hard and 2008 Joker? I know what we saw it but does that video make it obvious? 
+Also Chris dagget channel reacts to almost all videos. Chris knows if it was reported. therefore we have quicker reactions to what is reported but if a video is edited well?</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>{'rand1': 19468, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 32623}</t>
+          <t>{'rand1': 14884, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 58475}</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDE5NDY4LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMzI2MjN9'</t>
+          <t>b'eydyYW5kMSc6IDE0ODg0LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDU4NDc1fQ=='</t>
         </is>
       </c>
     </row>
@@ -1368,26 +1351,25 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> a long time ago most of the world used the most recognizable Roman Numerals, since that is what everyone knows.
-So the Emperor took it upon himself to have the Mark of the Roman XII Triangle Bead engraved into the coins, thus it has no history of anyone figuring it out, justifying why there is only a couple of different styles of tattoos. Basically, he just wanted</t>
+          <t>5/2
+[LINK]</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>4 comments,0 votes
-|ELIF
-|ELIF|ELIF|ELIF|ELIF|ELIF|ELIF|ELIF|ELIF|ELIF|ELIF|ELIF|ELIF|ELIF|ELIF|ELIF|ELIF
-Question: When visualizing scalars, should we always use " + alone or do we need to reference another symbol and where</t>
+          <t xml:space="preserve">
+In flock we have many ways of tagging content and we have all of the thoughts that work in a scenario. 
+Anywwyey, that would be handled through the ScreenRole (to be precise the ScreenRoles) and then EFF and the concoctions of it's eldest son, mouthy. But it is mostly around the issue of intertexter (to be precise inter</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>{'rand1': 70118, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 70602}</t>
+          <t>{'rand1': 48583, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 20137}</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDcwMTE4LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNzA2MDJ9'</t>
+          <t>b'eydyYW5kMSc6IDQ4NTgzLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMjAxMzd9'</t>
         </is>
       </c>
     </row>
@@ -1402,27 +1384,24 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>01/02/1991
-CAN Be 1??? |_|
-none... (”[X]“) CH
-That's it, thanks for clarifying!
-HILARIOUS</t>
+          <t>40 female references against imprisonment for nekkidness versus only 3 male references.
+Reply: because this is Japan where all the vics like tanks use a hyper naked almost feminines get up
+Reply: I have no idea and I think that it would be ridiculous because they would probably be banned from watching TV.But you could also start a campaign fighting that law (I know it's kinda quick but that super fast</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t xml:space="preserve">ive seen it done in movies multiple time, not groundbreaking but... the family and the production company did.  
-I think its to help with target audience appeal, the movie had a marketing plan for that "target" - girls. </t>
+          <t xml:space="preserve">It's certainly a legal issue, and I believe traveling between states is legal as well, depending on where you are from. There might be laws against it specifically for certain channels though, because it's more common for straight men to want to see women topless from time to time, especially on Victoria's Secret commercials when they want very explicit sexuality specifically for the male demographic. </t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>{'rand1': 77390, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 75212}</t>
+          <t>{'rand1': 38748, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 21060}</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDc3MzkwLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDc1MjEyfQ=='</t>
+          <t>b'eydyYW5kMSc6IDM4NzQ4LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDIxMDYwfQ=='</t>
         </is>
       </c>
     </row>
@@ -1437,26 +1416,23 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2 axial tides quarter Moon month and Full Moon month.
-On that, 1 degree of the axis of earth is around 23 million km from the Sun. And even more if you have had tides  and time zones change over the years.</t>
+          <t>° the tilt of the earth causes a difference between the East and the west face of the earth, if accompanied by an atmosphere with plentiful moisture in the air, rain falls. When you see a cityscape with bistres through the clouds and trees through the other side it is because of dust from major eruptions in the areas ok silicon valley, it is gold or pink kaaf because of dust in the external moons from karuvikon</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t xml:space="preserve">__________
-Problem: Three spare tires:
-All domains are relative so we couldn't use the word is because it relates to the question.
-</t>
+          <t>1) For the advantages of stability of the entire system. 2) Differentia Earth and Sun are different masses so the following diagram demonstrates why different axial or vertical movement for gravity force and sunlight affect earth 2) The most convenient reasons: 1) Earth rotates while Sun revolves 5 ° every 25 8 les
+2) Different masses, axial movement therefor gravity force slows down and angular velocity of sun displacement is slow decrease on</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>{'rand1': 17606, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 34546}</t>
+          <t>{'rand1': 73597, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 36629}</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDE3NjA2LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMzQ1NDZ9'</t>
+          <t>b'eydyYW5kMSc6IDczNTk3LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMzY2Mjl9'</t>
         </is>
       </c>
     </row>
@@ -1471,24 +1447,26 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1 NSF Longevity represents the minimum period of time between taking contents out of a refrigerated space and putting additional foodstuffs into that same space.  For food, they set this at about 4 hours.
-At room temperature, ice forms on the surface and some water vapour from the original ice sublimates off into the air.  The reverse process leaving water which can be absorbed back into the block of ice.  
-When the</t>
+          <t xml:space="preserve">
+That's a good question. Freezers are set to defrost overnight, but if you're like me and type zztime and grab the current date and do some math, then wait 8 hours, you're trying to open the freezer before it's still cold enough - but (like you mentioned) 
+The slight opening would warm the whole freezer within a few seconds
+  so you would be left with lukewarm or even warm</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Электрические замки имеют своих «бульдожировых двухяйлерок», подходящих не только  для людей помеченных синим и аква долго пьянствовать. With FREE affiliate banners and ridiculously easy commissions. Because АЗС лигробы донударавайте</t>
+          <t>1. High humidity makes that stuff stick.
+2. It creates a very annoying noise that is difficult to hear.</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>{'rand1': 29034, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 47302}</t>
+          <t>{'rand1': 94615, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 2748}</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDI5MDM0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDczMDJ9'</t>
+          <t>b'eydyYW5kMSc6IDk0NjE1LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDI3NDh9'</t>
         </is>
       </c>
     </row>
@@ -1503,33 +1481,25 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2 year ban from international competition
-Meaning of life isn't found simply
-Potential of a person is for making life truly purposeful.
-What should be the main purpose of a person's life?
-Answer: it's to achieve total happiness to God
-Must go in harmony with his nature
-Sin and drugs are caused by ego
-1. men has natural limitations
-2. therefore isn't important on which side you're
-3. importance</t>
+          <t>1. Leverage before Long-term proper training.
+2. Nobody really knows what the penalty for use of Performance Enhancing Drugs is.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t xml:space="preserve">37 athletes (37!) in the Sochi Olympics have tested positive for doping.  They marked it as a "deep fuckup" on their website.  None of the athletes has said that they did not do the drugs to try to improve their performance, but it was marked like that for casual misuse.
-Tend to follow with you.  Helps but as you age other benefits kinda outweigh it.
-</t>
+          <t>4 comments on'| | | Wordplay Beginner | Wordplay levels | | | Answer: i don't think that this is the right answer. The last word ('ouns' as in 'big'). It's not going to improve skill. It's going to boost confidence. You'll concentrate on one place and it won't do you any good. Read Essay on PED's Long-Term Health Effects
+Read Feedbacks
+I think this is not</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>{'rand1': 89518, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 751}</t>
+          <t>{'rand1': 27966, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 34597}</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDg5NTE4LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDc1MX0='</t>
+          <t>b'eydyYW5kMSc6IDI3OTY2LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMzQ1OTd9'</t>
         </is>
       </c>
     </row>
@@ -1544,25 +1514,23 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Basically, they are like roadside pay-for-plays (trucks, road-side signs, public announcements. like the one Greyhound corporate logo took the red out of "Greyhound" to make some corporate logo) dispensaries where, the user pays for "nugs".  The payer is responsible for the safe storage of the amount of cannabis. </t>
+          <t>✝☪ It's true what they say: stupidity is denial of geniuses. True, it was not from your question.</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>🤣 😂 🤣 I actually have no idea...
-It’s been my experience that the prices depend on what exactly you want to store and the size, but certainly not all the time. Check our Apartment Stories page as those guys might have better info.
-Hi @GarfieldLinux, thanks for your response.
-The property we looked at returned us a quote including annual rent of $3.60 for an 8 foot by</t>
+          <t>&amp;gt; &amp;gt; &amp;gt; So basically like a bank
+That is called a safe open, and if you haven't heard of it is almost always a bank/financial institution where you can put your money in a dormer box and they open it once a month to check its balance.  They don't give you the information to check the balance but they say they send you a card with the balance once a month.</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>{'rand1': 77165, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 6384}</t>
+          <t>{'rand1': 47313, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 91144}</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDc3MTY1LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjM4NH0='</t>
+          <t>b'eydyYW5kMSc6IDQ3MzEzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDkxMTQ0fQ=='</t>
         </is>
       </c>
     </row>
@@ -1577,27 +1545,24 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1) As I understand it, incest has a higher or equal probability of birth defects to older age given that younger populations have a lower life expectancy. 
-That being said, only a short sighted view ofcallback would regard reducing birth defects in older populations as an issue to be against. If the lower life expectancy could be interpreted as a risk towards the population at large, then it is more a political question</t>
+          <t>2 girls and 2 boys per pregnancy is ideal. The eggs dont mature and the fetus is healthy if both parents are healthy at about the same time.
+Two elderly parents are going to have different health and fertility issues compared to two younger parents.</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 For simplicity, I tried to make the prologue entirely a fairy tale. The lone sandal need not be part of the explanation.
-But there is :
-┌─────────┐┐ vetere └─────────┘┘ fleck ┐
-     +  ┉) thrice thrice   +-------------
-     Ô  </t>
+          <t>4+3=8 I 'll explain to you what is incest but that doesnt matter anymore You dont get it, I have explained but you make fun of it So, you are not religious so ask God Im on my way to work Right through the back door
+4. Adoptable children | |Here's it,''?’ There's those haters, huh? That's what religion is all about</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>{'rand1': 44057, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 93160}</t>
+          <t>{'rand1': 67832, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 99169}</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDQ0MDU3LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogOTMxNjB9'</t>
+          <t>b'eydyYW5kMSc6IDY3ODMyLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogOTkxNjl9'</t>
         </is>
       </c>
     </row>
@@ -1612,26 +1577,26 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1 - causes schizophrenia
-Because of illness (more precisely brain disease), sufferers often end up with odd situations in which they fail to be social by default whilst experiencing extreme social responses ("probably" schizophrenic), lack of social situation may set this brain disease off and start the processes that follow; obviously, nobody knows why this happens, but there are theories.</t>
+          <t>1. People generally like to socialise with their friends.  
+2. Our ability to plan for the future has more often than not back-fired on those who tried to prepare for a time in the not too distant future when humanity becomes a functionally extinct civilization. Planning for the future means that you will have to consider things and factors beyond your control.  
+3. The arts, when possible, tell stories based on human traditions and mythology.  
+4. The arts are often</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
           <t xml:space="preserve">
-What it means is that " distinct feature "; it complements of "stand-alone; " That why it's need of " "&lt;|ELIF|&gt;" :/
-There must exists a X civilization for testing federal X; and the technologies are highly matured until the space settlement work has been finished in the other civilization; so transporting to the Earth is the place to settle as an international project of mutual safety.  
-A: "ELIF" stands for "Expected observation of</t>
+Guzzles &lt;&lt;EMAIL&gt;&gt; &lt;https://web.archive.org/web/20150117011130/http://guzzlesin.com/wordpress/wp-content/uploads/2013/09/abi-wentz-guzzles-well.jpg&gt; Sent on: 2015-01-16 22:25:46 You could make my birthday as time const</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>{'rand1': 10288, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 37392}</t>
+          <t>{'rand1': 59418, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 90236}</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDEwMjg4LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMzczOTJ9'</t>
+          <t>b'eydyYW5kMSc6IDU5NDE4LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogOTAyMzZ9'</t>
         </is>
       </c>
     </row>
@@ -1646,31 +1611,25 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-#NULL
-The  as answer was originally shipped to everyone; instead of answering I left it hang out there for people
-A: For reference, you can find the source tree of elif.c from command prompt
-cd elif
-zsh: command not found: cd
-super: N_selection is 0
-pkgsrc.sh:14::17::strong-code-excerpts:3::/non-comprehensive</t>
+          <t>1) Quicker response to potential situations.
+2) Treating each major location (general headquarters? crime headquarters?) as its own "field". So things like the leader of a mob or a terrorist is simply "committed" to a particular field rather than being at the general headquarters unless something comes up they need to deal with quickly.
+There are still departments that visit places to support and/or investigate on behalf of the federal government, including DEA agents.
+But</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1879. The "Rampant corruption" in police - pretty much everywhere at that time!
-The new "exclusive agency" would investigate federal corruption in crimes, even go after bogus tickets from U.S. Marshalls, hence sign up as US Marshalls for their own department.
-In population-rich, modern America, the US Marshal is all but effectively a badge of insolvency - a Sherrif needs jobs,</t>
+          <t>69,000 federal employees – called "FIRSTSAVES" in the reports and press photos. This explains why only the "Super444". Description: The Office of Economic Stabilization has proposed a one-time public assistance package of one billion dollars to ensure that essential jobs could be kept in the federal government without harmful disruptions or adverse effects. The package would be administered through the Treasury Department's Financial Stabilization Division. Contra bill study confirmed</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>{'rand1': 49107, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 1547}</t>
+          <t>{'rand1': 43552, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 10761}</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDQ5MTA3LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDE1NDd9'</t>
+          <t>b'eydyYW5kMSc6IDQzNTUyLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMTA3NjF9'</t>
         </is>
       </c>
     </row>
@@ -1685,22 +1644,23 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1) Gaining the ability to attack at such low cost, since England's heavy manual labour was compensated for by its light heavy artillery. For example, in India two colonial governments had profits earned by the first from 8 to 50 times the cost of the second (1880–90). The unity of English forces and the strategic importance of India led the British political programme to revolve</t>
+          <t>1/ Britain paid for colonization. People in the colonies paid money to the British. Sometimes these people got some benefits in return.
+2/ The British had a LOT of very cheap salt that sold a LOT of slaves in the colonies. White indentured servants tended to stay and help make the colony work, so a lot could be made by replenishing the indentured servants every few years. People</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1. powerful navy and position of self ownership before america got there. the british also denied pirates rights to own their ship in order to help the colonies. 2. huge economies in both trade and mideast oil trade 3. colonists were well educated biblical scholars and a close match to the mindset of US founding father. 4. economy of scale with their manufacturing opened doors to competition and massive</t>
+          <t>40% of all land in the Americas is actually the colonial holdings of the British Empire. The British expanded their territory using the threat of force and proxies like Spain and the United States -- in essence, the same arguments used by the Spanish to transport American Indians across the Americas.</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>{'rand1': 29629, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 27793}</t>
+          <t>{'rand1': 50504, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 23268}</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDI5NjI5LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDI3NzkzfQ=='</t>
+          <t>b'eydyYW5kMSc6IDUwNTA0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMjMyNjh9'</t>
         </is>
       </c>
     </row>
@@ -1715,27 +1675,28 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2016-7-25 Vous connaissez cela ordre; dans le monde et chaque groupe d’etat est regulier, chaque group va devant se préparer de neurotrangÃ¨re Ã gauche Ã gauche)..Calculs billet scot butterfly umbrella fourchette de framboise et poivron</t>
+          <t>2||
+Books/Documents in reference to this task:
+1. The Wealthy Barber Returns, by David Chilton (Paperback-2004)
+2. Dave Ramsey (1987) Financial Peace Revisited
+3. Millionaire Next Door, by Mortimer Zuckerman (Paperback-2000) Steve Siebold (Paperback-20</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-- Buying assets
-- Real estate
-- Stocks/ Bonds
-- Private jets
-- I could go on.  Plus some really rich people even build whole towns, make donations, etc.  Wall Street is something to do, it's not just making money day in and day out.  Maybe you picked the wrong profession?</t>
+          <t>1. They dont manage their money. It just stays there.  
+2. It gets managed by people whom having a certain degree of understanding it. They mostly originate from  "elite" universities. 
+3. In 90s Eastern europe we have never seen and heard anyone with amount of money like this. I bet even in Russia the closest "incident" will be Aras Agalarov and</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>{'rand1': 96185, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 19599}</t>
+          <t>{'rand1': 28758, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 58100}</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDk2MTg1LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDE5NTk5fQ=='</t>
+          <t>b'eydyYW5kMSc6IDI4NzU4LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDU4MTAwfQ=='</t>
         </is>
       </c>
     </row>
@@ -1750,23 +1711,27 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>5 Hour Energy contains alcohol(distilled from corn) and high fructose corn syrup, while this presents an immediate danger to the quality of life, the apparent consequences of consumption are little more than headaches the next day and dizziness. Unfortunately these complications can be quite alarming to patrons, who, upon examination, may see a pattern of eyebrows akin to a human ski slope. To avoid potential lawsuits</t>
+          <t>5 He had a hold over research on the topic after a flurry of exposure concerning the safety. ROFL on 5. Any other product you are considering can not deal with "bottom shelf" material... it just doesn't worth it to them to do it. Similarly, "bottom shelf" product often won't hold/stay up to the 80 proof, meaning no by products...</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>5hrs isn't even a nicotine product. It's caffeine, sugar and a "natural energy boost"..and it's not allowed to market as 5hrs either.
-They didn't want to market it as a calm-down-in-a-tower option. It has a bad reputation that way.</t>
+          <t>5 Hour.
+Asked on May 7, 2013 under General Practice, Nevada
+Answers:
+M.D., Member, American Board of Physicians
+Answered 10 years ago | Contributor
+Your question is confusing because 5 Hour Energy and energy drinks have nicotine, though in very low amounts, e.g., 1 mg/can, because it</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>{'rand1': 64497, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 67744}</t>
+          <t>{'rand1': 75772, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 97364}</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDY0NDk3LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY3NzQ0fQ=='</t>
+          <t>b'eydyYW5kMSc6IDc1NzcyLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogOTczNjR9'</t>
         </is>
       </c>
     </row>
@@ -1781,22 +1746,22 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>80s music, was influenced by Rock, jazz, and soul music, y can hear echos of all these styles in modern day rock music, plz visit my blog at myspace.com/clearwordica Jan 24 2004</t>
+          <t>80s is a loosely defined term; it can mean anything from soft rock to dance-oriented pop to the intense synthesizer rock of groups like Foreigner; from new wave to funk or jazz rock. There are also the subgenres of "new wave", "power pop", "black music", "deep south soul", "new disco", "proto-metal", and so on. Add to that all the industrial, Western</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve">1980s is a period of music more so than a decade; the clothes, the dances, the television shows in advertising, the country music shot to death by the media, etc.  The 80s was the first time that the total influence of television was strongest outside of sitcoms.  There was music that in the main had nothing to do with the radio.  With that,Of genres were born.  </t>
+          <t>80s is a subculture in it's own right which many people are familiar with, which extends to slang used in different chatrooms and other forms of pop culture. The fashion and aesthetics is distinct and shared, if you lived in the 80s you could very much draw your own conclusions about how this worked. Maybe some others will elaborate.</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>{'rand1': 93636, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 43525}</t>
+          <t>{'rand1': 52207, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 82185}</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDkzNjM2LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDQzNTI1fQ=='</t>
+          <t>b'eydyYW5kMSc6IDUyMjA3LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDgyMTg1fQ=='</t>
         </is>
       </c>
     </row>
@@ -1811,26 +1776,22 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve">1) Muscle apartment is generally fixed.
-2) The outer 'coloured part' of the eye needs automatic correction of incoming light. If not corrected the eye starts showing signs of getting worse.
-3) If light is anyway unable to be subtly corrected automatically then it would change the general correcting power of the eye and it's very, very dangerous. Imagine prism sunglasses that shifted the colours to other parts of your </t>
+          <t>21|No, humans cannot make the appropriate eye-slighting muscles stronger, because they are cesspi|&gt;5SS"&gt; 3|ELUL - Lesson Twenty Other Topics Handwriting is different from writing in blank paper: we do not start the letter with a regular guide: swining of pencil and fingers passes on to and fro to the table, there is a dynamical flow of department that is coherent with the motion of handwriting</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>___________________________________
-|NDB.25||190||The fastest of whichSSB||HST||Before-After||Before and | |A temple.||Lastly the||Hoax||Choice@|| ____________solar system||UTM||None
-||||120|174||35|Fusion|Final|B|Yes|7|8||______________||O</t>
+          <t>2nd photo of eyelids</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>{'rand1': 31667, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 77112}</t>
+          <t>{'rand1': 43735, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 31997}</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDMxNjY3LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNzcxMTJ9'</t>
+          <t>b'eydyYW5kMSc6IDQzNzM1LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDMxOTk3fQ=='</t>
         </is>
       </c>
     </row>
@@ -1845,28 +1806,26 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1) Buy the Wrench The tacit understanding in America for more than a hundred years has been the middleman, who then promotes and displays the product, is the customer, not the manufacturer.  The retail price of the wrench isn't the manufacturer's price.  If the manufacturer reduced the wrench to minimum wage, or screwed it with a high price, one could argue that discouraged them form doing business together.
-It doesn't seem to make sense</t>
+          <t xml:space="preserve">
+They can.  Think of the cars as a bunch of attendees at a convention mostly seated in the same room.  They each want the same brochure, someone has to deliver it for them.  Go buy one car; the manufacturer has to make another car for you. Same applies to an actual showroom.  
+Now imagine you not having to buy each car.  If I buy one car, you buy one car.  We can buy all the cars we want at wholesale at</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3D trucks on the internet
-# The Sdx1000 3-D Truck - Tarson Eliassen
-# 3D-SX1000, The World's First Internet-Connected 3-D Truck - Tarson Eliassen
-# Elon Musk interview: VW takeover,pounders,children
-# VW-Gaggle, Stuttgart, story, Late night special
-# VW cost/opp</t>
+          <t>1. Because they don't want to bother with detailing, state licencing, etc. 2. Because they don't want to deal with dealers that won't pursue warranty problems.
+Question: Given a mounted display (e.g. Elgato EyeTV Docking Station), what other kind of display could be used?
+Answer: Argh, can't remember. I think I recall the TV company that makes the frame gave me a link to a patent for it,</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>{'rand1': 23777, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 11226}</t>
+          <t>{'rand1': 61131, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 4700}</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDIzNzc3LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMTEyMjZ9'</t>
+          <t>b'eydyYW5kMSc6IDYxMTMxLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDcwMH0='</t>
         </is>
       </c>
     </row>
@@ -1881,28 +1840,24 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">1) Because beer is inexpensive and voluminous. 
-2) Because it makes sense for a provider of said drinks to not compete for purchase of those drinks. 
-3) &amp;gt;But dont well companies naturally compete for sales that are already there? </t>
+          <t>1 Here it comes: It's because a company can't have competing goods or services. A "generic notion of interdependence" might add credibility to the fact that some firms are required to compete in different goods and services and no particular resource can be identified as essential for their market survival, but on the other hand this weakens the concept by mildly constraining the occurrence of</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1)Thankstrudelpie de Chambour drew a beautiful analogy.
-2)The same reason why you can choose
-Bud Light or Miller Light over Coors Light or Budweiser.
-EzraMitIN: For the consumer, what are its main concerns?
-Tal Barak: The main concern is the healthiness of their products. The</t>
+          <t>1. Millers Light is a product of the soft drink companies, not an independent one.  
+2. Coke, Pepsi, and 7 up all have similar taste.  Coke Pepsi 7 up.
+3. There is little DIFFERENCE between Coke, Pepsi, and 7 up. "my favorite is the favorite" is a</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>{'rand1': 9415, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 10134}</t>
+          <t>{'rand1': 44602, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 27545}</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDk0MTUsICdkb19zd2FwJzogVHJ1ZSwgJ2Fuc3dlcjEnOiAnM0JfY3AtMjUwMC5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAncmFuZDInOiAxMDEzNH0='</t>
+          <t>b'eydyYW5kMSc6IDQ0NjAyLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDI3NTQ1fQ=='</t>
         </is>
       </c>
     </row>
@@ -1917,32 +1872,24 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>5:22 |ENUM|&gt; Caesar cipher
-4:17 |INPUT|&gt; basic unit operations
-12:17 |BIT_ORY_LT|&gt; CPP Boolean Constraint Package
-Introduction to Boolean Constraint Package
-7:35 |BIT_ORY_GT|&gt; CPP Reversal Checking
-Dijkstra与其他
-- Beck 2005: Избранные задачи
-7:25</t>
+          <t>1 it's cute, 2 to open the door vadimbredik, 3 I do believe this guy is sick</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t xml:space="preserve">1. When we say "sofa" we automatically assume it's stationary. 
-2. To a human it challenging sofas looks as "random faces moving in those awkward patterns".
-Suppose you have 10 moving sofas. Then if you observe 10 x 10 x 10 = 1000 faces. If you observe pixel by pixel, logarithmically you wouldn't see a pattern at all.
-</t>
+          <t>1. The Moving Sofa Problem is considered non-solvable, as no approximation algorithm has been found that achieves the construction time goal of O ( gn + +n) for all n0.2,... 0 to g &lt;=14, 0 to 0
+Notes: (0.2 = Average of [0 to 1])
+G = (2)n0, (0)n1, (1)n1/3, (3)n</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>{'rand1': 87996, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 65915}</t>
+          <t>{'rand1': 32063, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 12296}</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDg3OTk2LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY1OTE1fQ=='</t>
+          <t>b'eydyYW5kMSc6IDMyMDYzLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMTIyOTZ9'</t>
         </is>
       </c>
     </row>
@@ -1957,29 +1904,26 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1) if you are not paying any taxes, you should probably figure out if you need to be paying taxes.
-2) there are millions of households in america that pay no income taxes because they get a large chunk of their income in the form of refundable tax credit from the IRS.  This gives them all sorts of nice additional money, and so it is a well known get rich quick scheme to get a job at an IRS office, declare some bogus income,</t>
+          <t>47% of people in the US pay no federal income taxes.
+80% is almost 3/4 of all Americans in the US.
+47% does NOT include Savers, who produce barely any income and certainly pay no tax on their savings, unless they take out loans against their pension savings,, which they usually do in retirement when they are facing financial hardships that are related to locating alternatives to pensions.
+80% of a county'</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>47% of people in the US do not pay federal income tax, but it’s rebated to them.
-Why is the US federal government taking taxes from 2 trillion US dollars spent?
-Here are the reasons:
-- you would expect some of budget to come from the people who don’t pay federal income tax:
-- subsidiar quality moocs of free universities
-CONUS are subsidies (tax breaks) explicitly given to needy citizens
-Th</t>
+          <t>47% in the US: is not exactly accurate. It's 47% not paying enough taxes. 
+The government limits how much they take out of your paycheck. There is a deduction for every paycheck. You pay less or more than that percentage depends on how much you make and how much the Company sweetens your stimulus check with. So since each company rebates the government a certain amount for every worker, a lot of people are getting money back</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>{'rand1': 39926, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 96406}</t>
+          <t>{'rand1': 99731, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 59858}</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDM5OTI2LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogOTY0MDZ9'</t>
+          <t>b'eydyYW5kMSc6IDk5NzMxLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDU5ODU4fQ=='</t>
         </is>
       </c>
     </row>
@@ -1994,24 +1938,26 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>951 Questionable questions. 79 judges. 54 debates. $1644 in prizes. Users’ top vote: Numberphobic: 17
-Weekly Taboo: coq au rationstable. Box of TalequoisCopy? | 1990 | Sardine soup | Redneck sounding name for the North?
-RCS’ (Hard/Easy) | #534 Jeff vs. Dave | Week</t>
+          <t>2017/11/02 12:58
+We do lots of CFÜ images now that highlight murky tie-ins.
+Border House – Hustler blog, now being torn apart by posters.
+Frameshift -Buttfloss post, whole lot of noodle salads and kebab, but no pockets.
+Informative: Should Joseph Gordon-Levitt save you? Although: why should we ever trust</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>500 unique users. Either way, I suspect that the army is being overwhelmed. What I suspect is that users see this nesting question and immediately start /u/ev-bakugan</t>
+          <t>15 minute banning spree across the top ranks of r/thebutton. The R2P act was also in effect, but whatever. A pyramid of bots was probably the biggest issue.</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>{'rand1': 67533, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 9992}</t>
+          <t>{'rand1': 81382, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 65387}</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDY3NTMzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDk5OTJ9'</t>
+          <t>b'eydyYW5kMSc6IDgxMzgyLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY1Mzg3fQ=='</t>
         </is>
       </c>
     </row>
@@ -2024,21 +1970,28 @@
           <t>When I plug my nose and blow air really hard, my ears "pop". What is actually happening?</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tinnitus agression = collagen stuff in the ear. When you rupture the ear the fluid builds up &amp; when you poke you ears with pressure, it makes sure of yourselve.
+see ear popping as your brain generates two thoughts at the same time: a high pressure burst in the middle of your ear, and a high pressure spray at the invading air from outside, moving your head to the middle of your body.
+</t>
+        </is>
+      </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2 blue tubes
-Whenever you take a deep breath in through your nose, the fill up your lungs. As you hold your breath, the air that was in your lungs, now left in your nostrils. (Although when you turn your head the static pressure on the inside before you take a breath is greater the surface pressure, the atmospheric pressure is meaningless.) Pressurising the blood in your system means that it is almost all going into the lungs</t>
+          <t>14:13 Question: What does the color below mean? ( Used option /s dark )
+Answer: ======================================================= Hard question, hard answer... 14:15 Question: What does this error mean?
+Answer: Has changed post and you will not see the error message......... 14:11 Question: What color is displayed when you charge the rollerball stylus</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>{'rand1': 79930, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 30246}</t>
+          <t>{'rand1': 39236, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 91594}</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDc5OTMwLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMzAyNDZ9'</t>
+          <t>b'eydyYW5kMSc6IDM5MjM2LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogOTE1OTR9'</t>
         </is>
       </c>
     </row>
@@ -2053,34 +2006,27 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> filming that sets a person’s face
-with flickering oil paints and
-stuff that collects on knobs,
-so they can see
-what’s coming after a traumatic experience.
-The targeted fabric rose seamlessly into the air, for
-Let’s: Have a get together / Join us soon
-Fin: EASTER 2020
-(CB Nowrange. Singers, Cursing #1, Wore my Pajamas to Work)
-</t>
+          <t xml:space="preserve">t h e w r o n g o f t h e w o r l d.
+People clap their hands, not because they want others to think they haveiously good taste, but because they feel accomplished for finishing a race in a decent time. 
+The feel recognition endorphins kick in, in addition to the natural physical effects of losing 50-150 lbs of endorphins per week. </t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-In the aristocracy of ancient civilizations, clapping your hands was the ultimate form of appreciation. It was reserved for the nobility and was a rare act.
-The act of clapping your hands ended up being adopted by ordinary folks, and its constant use is a signal of high regard.
-</t>
+          <t>14. Designated number of topics are prepared on the same form (see below). All of the questions are straightforward and uncomplicated. Use the system transportation to move from one topic to the other. Some transitions are allowed.
+&lt;|ADJ|&gt;IT development Not all developers are equal. ——————————— self-learn many knowledge
+| run his own large IT m | he is very good programmer —========================
+| Establishing convenience stores | the research needs to be monitored —</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>{'rand1': 78519, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 33327}</t>
+          <t>{'rand1': 68863, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 79728}</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDc4NTE5LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDMzMzI3fQ=='</t>
+          <t>b'eydyYW5kMSc6IDY4ODYzLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNzk3Mjh9'</t>
         </is>
       </c>
     </row>
@@ -2095,26 +2041,27 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2¢: Weird perfumes :: MustyMoo's Comment: 2¢: The must has to go.
-Who doesn't like to try things off brand?
-Answer: 61% of the US public.
-Source: Daily Finance :: 89% of consumers are unhappy with the service they receive from existing brands.
-"Why?" what is it that makes us dislike a brand so much that we won't even try</t>
+          <t>1) You need to build up bladder capacity by taking small amounts of fluids during the day or you risk not being able to go when it's really necessary.
+2) Hiding increases the opportunity for fatigue and bodily injury.  So not only will you be desperate to get to and get out of a babyi house, you will be fully exhausted.  That vomiting may be one of your unique physical defenses against predators combined with the scents</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1) mother and I would play hide and seek outside and your father and I would hide in the corn a-mess..when we heard you coming we'd all (your sister and I) come out and wish it was time to play mother, father, son and I...then we all hit the corn canadaguns..while your sensei stood out there since she thought we were playing hide n seek and could see us yeah we did that...(l</t>
+          <t>NEHW_ADa|_|&gt; |DFAD|vs
+|MDA=&gt;|GFAD|tk^
+&lt;|&gt;SDFER|FL^|&gt;PDE
+PGA|9|&gt; 9PP
+QFT|&gt;</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>{'rand1': 63743, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 66057}</t>
+          <t>{'rand1': 22628, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 13811}</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDYzNzQzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY2MDU3fQ=='</t>
+          <t>b'eydyYW5kMSc6IDIyNjI4LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMTM4MTF9'</t>
         </is>
       </c>
     </row>
@@ -2129,25 +2076,26 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1) Different flowers when replicated into flowers, produce varieties of the same flower, some with smaller and fewer, others with larger and more. This is part of the sexual reproduction method these flowers use (pollination) 
-2) I'm not sure how they all get recognized and go to make honey (i.e. the ones that are used) vs the ones that aren't. I think those that are are the ones producing the most, but this is really just a</t>
+          <t xml:space="preserve">100% breed (group of bees that mate and produce more bees of the same species.) Some varieties of flowers also give a distinct flavor to honey, based on the pollen the bee picked up on its way to the flower, and what kind of nectar it found when it arrived. Not all flowers have different nectar, but some have slightly different flavors based on a more different combination of pollen and nectar. 
+</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> эффект трендатового поведения (стабилизация сиры), если я скопирую из Wikipedia из интернета, а не из других источников
-Feels weird when seen on live news for the first time. @hwarefields
-Hатфа-хатфарта выполняется когда BBC выписка выгляди</t>
+          <t>1, 7, 11, 16, 25, 48, and 112
+The Multi-Sighting In The Midst Of The Picture square is an addition to the Wild West Trail.
+Three pairs of opposite words form the six squares in this puzzle: STOP | &lt;&lt;&lt; CRISS-CROSS | CONTRAST &gt;&gt;&gt;. Notice that all three pairs are forced upon you in a 3-d cross.
+Answer</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>{'rand1': 13828, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 67536}</t>
+          <t>{'rand1': 7510, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 12579}</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDEzODI4LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjc1MzZ9'</t>
+          <t>b'eydyYW5kMSc6IDc1MTAsICdkb19zd2FwJzogVHJ1ZSwgJ2Fuc3dlcjEnOiAnM0JfY3AtMjUwMC5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAncmFuZDInOiAxMjU3OX0='</t>
         </is>
       </c>
     </row>
@@ -2162,32 +2110,28 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>13
-Question: 18
-1 | late | 2 | 4 | 3 | 5 | 6 | 8 | 7 | 10 | 11
-| 12 | 13 | 15 | 16
-8 | 9
-13
-Name: ______________________________________
-Class: _____________________________________</t>
+          <t>666666666
+BOARDS and PUBLICATIONS Camille Stro purplefeather.net
+Questions to keep in mind 344619857266206
+Kingdom of Heaven, a relationship with God Float like a Butterfly; Stiny like a mosquito
+Divine Affirmations 7508455239
+How You</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>t/s was Peukka, and he had the better explanation since you used it. But here is a second take from Lightbender, who has a good hint on what ache is:
-"whats good
-The chemical changes in your hair and teeth are caused by the open tubule systems, which take stress and heat as a product.
-Well, in the cantaloupe situation, your enzyme got activated first</t>
+          <t xml:space="preserve">
+Since you asked using the entire scope of this amazing amazing Supreme Court of America film as an answer, Liam has a point.</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>{'rand1': 71540, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 59382}</t>
+          <t>{'rand1': 42417, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 23954}</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDcxNTQwLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDU5MzgyfQ=='</t>
+          <t>b'eydyYW5kMSc6IDQyNDE3LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDIzOTU0fQ=='</t>
         </is>
       </c>
     </row>
@@ -2202,28 +2146,28 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1851940870
-Get the Authority on Business Services. Microsoft Gold Certified Partner.
-How does a Skinny Budget help you stay fit and economically?
-Surface apps Mango Runtime updates it's just like Illumination.
-His drive with Surface RT someone object to much real, Sadly demo graphics.
-How Sandisk use the cloud. your feedback please messages, RT.
-Everybody going: "Cruza" is Mango care Developer Tool is</t>
+          <t>25
+#10 | Laser Rifle, Question | OFFLINE
+Someone posted the link to this website (I think it's doomedwave.com) but I can't read Japanese. The images at the bottom left are chess pieces and the images to the right are boxes of some sort. Pretty crazy.
+Question | Purim | ONLINE
+I love when the final moments of pop songs wrap up in the music video with symmetry.
+Question | Pulp Fiction</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1. They are from the same company (now owned by Apple) that makes the "Chargerspeaker" for laptops and you can use your charger to charge or listen to music to/from it (depending on the type)</t>
+          <t xml:space="preserve">
+Cables are designed from the outside away from the metal conductors that themself use to carry electric current. These are corrosion magnets which can bypass grounding and allow even popular metals such as aluminum to conduct taking an awful lot more amperage and charging at electron speeds people no longer understand. </t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>{'rand1': 8925, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 76427}</t>
+          <t>{'rand1': 33649, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 41687}</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDg5MjUsICdkb19zd2FwJzogRmFsc2UsICdhbnN3ZXIxJzogJzNCX2Jhc2VsaW5lLmFuc3dlcicsICdhbnN3ZXIyJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ3JhbmQyJzogNzY0Mjd9'</t>
+          <t>b'eydyYW5kMSc6IDMzNjQ5LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDQxNjg3fQ=='</t>
         </is>
       </c>
     </row>
@@ -2238,29 +2182,28 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Personal experience: if there is no more sexual stimulation in a relationship, et voila, the spark dies. 
-When a man and woman are both 30 their sexual relationship will be different than 30 years in and two women because at 30 you have seen a lot more than you did when you were 20 and women will last longer and keep you interested longer, etc.</t>
+          <t>3 step math…..
+&lt; |lol ;)| doug b ^^pyro^&gt; I have a zebra fish.
+Tell me more about it.
+What’s in the trunk?
+Da guy falcon f
+Oh wow… 0.724… by creativeness and freedom? Yes, that was what my very first college instructor, lo these many years past, used as her grading criteria</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-&lt;|ELIF|&gt; Tolerance: the opposite of intolerance. 
-&lt;|ELIF|&gt; Alpha Males: High status males who have the opportunity to demonstrate these traits in order to pass on genes 
-&lt;|ELIF|&gt; Altruism: selfless concern or unselfish care for the welfare of others 
-&lt;|ELIF|&gt; Amnesia (distinct fields of memory): 
-</t>
+          <t xml:space="preserve">13 months old so ya it's ambiguous but if I had to make a guess it's because you didn't previously find the elderly as interesting. 
+Not anything specific to women, just life in general. When faced with something new you generally desire to learn more about it. And the more the better. </t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>{'rand1': 87010, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 66199}</t>
+          <t>{'rand1': 81292, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 84207}</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDg3MDEwLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjYxOTl9'</t>
+          <t>b'eydyYW5kMSc6IDgxMjkyLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDg0MjA3fQ=='</t>
         </is>
       </c>
     </row>
@@ -2275,24 +2218,26 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1) old tech, i.e., OLD planes. Plane damage is rare.
-2) security. If you are a terrorist you don't want people tripping over broken seats or badly done wiring when looking for a weak point in the electrics. We know that recording the actual black box can't be done without causing a problem with the plane but we can still check that</t>
+          <t xml:space="preserve">1) These boxes record the plane's flight data (speed,...), while recording into them. Wiring is not allowed on planes. 
+2) In the US, the air traffic control relies on this data in emergency cases or crazy crashes when people don't quite know what happened. </t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1. Since these claims are literally true, and 2. Because these claims damage the incipient conversion in a normally peaceful person to a maniac.)
-References: Free from the Classical Model Philosophy Textbook:Quantum Foundations textbook: Classical Foundations, there are other major applications of quantum theory. "Table of contents" on scientific web site known as "European</t>
+          <t>23.6 Joules, for example. Let's perform some number crunching. The air speed function, of course is:
+{{.9,controller}}
+Physics was the answer to heterogeneous networking in ebooks. Equations really are neatest when seeing them in FPGA.
+So, we have slight relation between energy and mass. Meaning the energy/mass density</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>{'rand1': 95904, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 87917}</t>
+          <t>{'rand1': 60315, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 24388}</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDk1OTA0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogODc5MTd9'</t>
+          <t>b'eydyYW5kMSc6IDYwMzE1LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMjQzODh9'</t>
         </is>
       </c>
     </row>
@@ -2308,29 +2253,26 @@
       <c r="C55" t="inlineStr">
         <is>
           <t xml:space="preserve">
-"Teh difference between alligator and crocodile is that crocodile..... "
-Patrick
-A: The form of the original questions is corrected. 
-A: The sensation of Crocodile Tears.
-*
-*A drop or film of saliva that is visible to accidental debtors.
-*Trademark. The film of liquid membrane encasing the</t>
+Alligators are a primitive version of a crocodile and share a lot more in common with fish and other reptiles. Crocodiles evolved from members of the turtle order (along with the dinosaurs). Many of the adaptations present in both animal groups are related evolutionary casualties, which means they're shared between them. 
+Don't lump them all together though. </t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> the alligator does not lay eggs, its reproductive cycle is very different. Crocs lay eggs &amp; can spawn 300 per season &amp; alligators lay eggs &amp; can spawn 72 per season.
-The other big difference is gators live in fresh water &amp; crocs in saltwater</t>
+          <t>1. ALLIGATOR - 2. CROCODILE 3. HELIX -11.
+Evolution of the DNA based on rules and the ratio of the amount of double-stranding:
+1) What are the components that are explicitly mentioned in the paper by Fisher and Haldane for the probability?
+2) The above mentioned paper mentioned that the probability is the sum of all the contributions to the title</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>{'rand1': 48432, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 39826}</t>
+          <t>{'rand1': 45561, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 27588}</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDQ4NDMyLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDM5ODI2fQ=='</t>
+          <t>b'eydyYW5kMSc6IDQ1NTYxLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMjc1ODh9'</t>
         </is>
       </c>
     </row>
@@ -2345,28 +2287,29 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>8track are a fad.
-TL;DR Cursing is now a fading fad too.</t>
+          <t>1. Vinyl lasts longer making them more practical
+2. Vinyl is better on almost every other technical and aesthetic level than the new digital material equivalents. In particular he sound reproduction of vinyl doesn't colapse as significantly as is the case with both mp3's etc
+3. The physical properties of vinyl are attractive to record companies. They are easy to produce (and upkeep cheap) and to sell as</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.vinyl was popular, prices were cheaper than cassettes/8 tracks
-2.the electronic repressing possibilities can't match other records
-B.CHECK |D| Sort of bumper stickers, "yeah I'm with "the other side" mostly: alternative views of the 2000 election.
-C.OFTEN
-D.RADIO
-Question: Men hold "man</t>
+          <t>3 blocks of Full Research Analysis for this 5 minute question.
+14.5 blocks of Full Research Analysis for this 24 minute question.
+15.3 blocks of Full Research Analysis for this new 5 minute question.
+15.1 blocks of Full Research Analysis for this new question.
+10.2 blocks of Full Research Analysis for this new question.
+5.1 blocks of Full Research</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>{'rand1': 36530, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 78988}</t>
+          <t>{'rand1': 30098, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 45087}</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDM2NTMwLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNzg5ODh9'</t>
+          <t>b'eydyYW5kMSc6IDMwMDk4LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDUwODd9'</t>
         </is>
       </c>
     </row>
@@ -2381,25 +2324,27 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>13.|MANY|ANSWERS|&gt;&lt;|ELIF|&gt; Do you know how many answers there are to the Laplacian problem?
-Solution de la problème de la lavandiere: Infinitely many answers...
-MODEL C:|ELIF|For possible matches, A-Z, 0-9. Symbols &gt;, &lt;, in, Ny and Xp are assigned letters and numbers within the</t>
+          <t xml:space="preserve">30 year old here, so not sure if it's different amongst young people, but to me I always feel generic allergies- especially tree pollen which I'm always getting in April even though I live in the East Coast (definitely a return from the Midwest).
+Also sleep on a hardwood floor. Made me even more stuffy the first night I slept in his flat, but at least I had my own bed at my place.
+</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-People sleep in different ways on average, therefore with different forms, amounts and wavelenghts of nasal/pharyngeal mucous. Some will be filled with gunk all the time, others will be out of the way kinda, and others will just be ravenously clean like giraffes after a carmine hunt.</t>
+          <t xml:space="preserve">1.|Because I sleep on a urban fox|2.|Because I cannot say no first thing when you awake|3.|Because I have a tomboy living in my stomach|4.|Because I have common sense| 135 Views Add Answer42 Answers. 54 Views Add Answer2 Answers · 135 Views.
+Other Popular Quizzes
+Sorted by: Active | Best | Most Viewed
+</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>{'rand1': 3450, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 83642}</t>
+          <t>{'rand1': 60298, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 73604}</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDM0NTAsICdkb19zd2FwJzogRmFsc2UsICdhbnN3ZXIxJzogJzNCX2Jhc2VsaW5lLmFuc3dlcicsICdhbnN3ZXIyJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ3JhbmQyJzogODM2NDJ9'</t>
+          <t>b'eydyYW5kMSc6IDYwMjk4LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNzM2MDR9'</t>
         </is>
       </c>
     </row>
@@ -2414,25 +2359,30 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1. The 2.4 GHz processor has 2 cores 2. The.4 Ghz processor has 4 beautifully designed cores.Updated On: 2019-10-20 10:34:14 UTC
-Could a bear from today be flying first class?
-The web crawler Kosada is randomWhat mean HTTPS in this picture? | lildude | youtube.com</t>
+          <t>2.4 Ghz CPU can't be more powerful than 2.4 Ghz CPU
+Kevin
+I tried to write 'Mumbo logic' to post a comment but
+the blog wouldn't accept it. So now is the time to
+get another free up-grade to a richer OS and
+better memory.
+Nice posting manpowergan.
+Here is a link to "Celsius" a free software</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2.0 GHz isn't a dumb thing that the designers decided to do, it's part of the standard. But really, ghz rating is a measure of the raw power, not a measure of what one can actually do. Theoretically, 2 Ghz will allow the treatment of more data in a shorter amount of time. 
-For example, the CPU of a one year old computer may have a</t>
+          <t>10 bits is pretty powerful. But with so many trinkets on a single board, they can only shine so bright.
+[Processor Galleries: Intel Core i3-3220 3.30GHz]([LINK]/)</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>{'rand1': 21977, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 11178}</t>
+          <t>{'rand1': 61330, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 393}</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDIxOTc3LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDExMTc4fQ=='</t>
+          <t>b'eydyYW5kMSc6IDYxMzMwLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDM5M30='</t>
         </is>
       </c>
     </row>
@@ -2447,19 +2397,28 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>84 percent of respondents got paid or got some sort of reward for their research
-Quote: "!=78 | '14,_/ | |,--' \`_='/ / | | (o........\ | _( '' _ =o/,,0. 8\ | _'/__ный_-6\_ 8"| | \ --',| '`-_)=_-_-_=-_(__</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr"/>
+          <t>10p-1: not usually; 20p-2: every once in a while; 30p-3 = rarely
+Question: What proportion of chemists usually have sick leaves?
+Answer:? (might be ~0.5)?
+Question: What proportion of biologists would sign to work under their own contracts (not under the University) if given the chance?
+Answer: ~ 1/3?
+Question</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>6-5 law shields discovery projects, but a lot of the experiments are conducted by the McGill Research Board  which provides funding for graduate students.  Obviously it would be unrealistic to hope for a patent, because it would typically be a simplification of what has already been done and documented.  Thus the motivation for funding theses  students would be to advance research in the field. This means more researches can be made.
+that</t>
+        </is>
+      </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>{'rand1': 89062, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 20255}</t>
+          <t>{'rand1': 54586, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 15897}</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDg5MDYyLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDIwMjU1fQ=='</t>
+          <t>b'eydyYW5kMSc6IDU0NTg2LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDE1ODk3fQ=='</t>
         </is>
       </c>
     </row>
@@ -2474,27 +2433,26 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t xml:space="preserve">    They want more power to make their currency cheaper or more expensive.
-It's in Russian's economic interests to pin Ukraine down to their economy, helping the currency work cheaply for themselves. 
-As a direct invasion takes Ukraine further away from China and the West...essential if they want to connect Russia and China up. 
-</t>
+          <t>4 of them.
+Quad 18 could have ended at this point. It would have signaled a large win for Team Putin. Instead, they’re gonna keep going.
+Now, I’m not usually against detouring a couple space-command points. The move just happened for complex reasons.
+The thing is, though, Team I.R.A.C.K. seems to have calculated it correctly. They see the weak point on the continent. They don’t</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1 The U.S. is battered, feared in the world.
-2. | PLAY DONALD EPI-MIND FOREIGN POLICY SERIES# 25 Questions | Russia: Forming A New Government
-| After pushing himself from a controlling share of a coalition between the conservative regionalist Party of Regions, the pro-Western populist Union of Right-Wing Forces, plus Communists and liberal Democrats, former president and oligarch president</t>
+          <t>tl;dr: Russia's military decision was predictable, but Russia's political objectives were not. 
+The Crimea is strategically important. It sits right next to Ukraine, and only about one fourth of Ukraine is occupied by the Russian military right now. It also overlooks several ports, and if Russia had at least 110-100,000 troops in that territory they could control 2/3 of Ukraine. More importantly, Crimea is very important</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>{'rand1': 27936, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 10653}</t>
+          <t>{'rand1': 89413, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 31389}</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDI3OTM2LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMTA2NTN9'</t>
+          <t>b'eydyYW5kMSc6IDg5NDEzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDMxMzg5fQ=='</t>
         </is>
       </c>
     </row>
@@ -2509,28 +2467,25 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Eligibility Verification:  US citizenship status is to be administered according to the Naturalization Code
-The Congressional Budget Explanation (CBO):  Assists members in developing bipartisan vision and consensus on matters such as federal budget, appropriations, and health reform legislation
-The Congressional Research Service (CRS):  Makes historical, statistical, legal, and budgetary studies of legislative activities
-The Congressional Resources Council (CRS): The Congressional Research</t>
+          <t>12 years after Reconstruction ended and for half century before the global Depression NEVER EVACUATED after returning to power the majorities embraced GOP proposals to dissolve the Democratic party through party purge. 
+Ku Klux Klan linked voting territory was established,  sodomy laws in every state was passed,  the notorious Jim Crow laws allowed no white people to be in the same room with blacks, and known rapists localized in</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1860, 1870, 1880, 1912, 1932
-That was a cycle. Democrats grew popular comparatively stagnant.  The cycle then flipped for another 120 years. Finally Republicans began a cycle of losing elections and then painting their opponents as limtited growth socialists.
-This changed in 2016 when the college educated, economically</t>
+          <t>1|ELIM|&gt; With name pins. If you're so much a slave owner why didn't the Southern States get that name back?!
+Answer: 1|ELIM|&gt; With mouse pads. Clearly you were a slave owner.
+Answer: 1|ELIM|&gt; Let's ask Nero how did they get out. He(all semblances of good men) demagogued the poor, put up</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>{'rand1': 47623, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 31738}</t>
+          <t>{'rand1': 84048, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 68302}</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDQ3NjIzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDMxNzM4fQ=='</t>
+          <t>b'eydyYW5kMSc6IDg0MDQ4LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjgzMDJ9'</t>
         </is>
       </c>
     </row>
@@ -2545,25 +2500,28 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>tired... dumb if you recalled that in your sleep
-Your alarm is ringing, time to get up. 
-New day, school, work, or whatever.</t>
+          <t xml:space="preserve">1) Evolution - when you sleep you are effectively doing nothing, when you are awake you tend to be more active by default
+2) Lack of immediate reward
+3) Being awake results in better memory and memory takes longer to process
+These four things combined to delay need for a life strategy </t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>1.1 out of 3
-&lt; |-- limelight |-- mulligan |-- ElibsonClan |-- ilicio.consulatu.nomen |-- ecosystem |-- outlook |-- periphrastical |-- aswiculturama |-- moralist |-- energistic |-- busy |-- ecofisherlandz</t>
+          <t>_____________________________________________________ _____________________________________________________Posted in Writings | Leave a commentPosted in Writings | Leave a comment
+Listen to _________________________________________________________ _________________________________________________________
+About Mamihlapinatapai
+Mamihlapinatapai: a Jargon File entry about a term used by</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>{'rand1': 35731, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 13914}</t>
+          <t>{'rand1': 97352, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 86907}</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDM1NzMxLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMTM5MTR9'</t>
+          <t>b'eydyYW5kMSc6IDk3MzUyLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogODY5MDd9'</t>
         </is>
       </c>
     </row>
@@ -2578,23 +2536,26 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1-Bile0-Mr. Taube4-President Barack Obama2-No pinning in the futureTMP: Not a Realist
-1-Jaime Westwood3-Quizilla3-xoxoVicky9-You need to be more hydratedNancy: 2Terroduggie ans 1-Mr Taube3xsweetstarNOW Playing:</t>
+          <t>☹
+☹ The liquid inside your stomach is called "viscoelastic" (viscol = fluid plus elastic). Stomach acid is 1000 times more acidic than regular mild cleanser (surfactant) in your throat (it's also why drinking carbonated beverages is bad for our teeth).
+☹ In order for smooth swallowing, the throat dries</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1) Not possible to unfreeze your throat 2) Possibly to simple throat burn from acidic drinks, Caffeine, and/or alcohol 3) Possibly other factors</t>
+          <t xml:space="preserve">
+First, my Digestive Physiology book, says that that when something solid remains in your throat for long durations, it can make you feel tired and dizzy.
+Secondly, you might be consuming large quantities of coffee/black tea, which are strong stimulants that make you thirsty. If you continue consuming that much you will become dehydrated. This, in turn, causes</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>{'rand1': 29942, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 6571}</t>
+          <t>{'rand1': 54032, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 14523}</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDI5OTQyLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY1NzF9'</t>
+          <t>b'eydyYW5kMSc6IDU0MDMyLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDE0NTIzfQ=='</t>
         </is>
       </c>
     </row>
@@ -2609,24 +2570,22 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>02:46 - Find some focus in the bedroom and around your house. Your subconscious uses around 80% of it’s energy. The crystal works in your 4 layers of energy to keep you feeling peaceful
-tube 10:04 - This performer isn't afraid to show her bare chest or booty! Pssst... sub to our channel for tons of sex, reviews, and Shoutouts to our best performers</t>
+          <t>1954 Television interview with Fred Allen talks about how he feels when someone is standing behind him. Perhaps that's the famous clip.</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2 reasons to be behind you: Sight + Dreamer.
-When you sense someone being behind you, one of those reasons is likely on the move. You can either spot them up and see that they are walking past you (or very near you) or detect that they are moving up and down the stairs/stairs from a shadow. If one of these senses are triggered, I.e. you see someone moving but you are already awake, your</t>
+          <t>20:35 DPGK |NNAME [: Question: I understand that if I felt a "worry or unease" somewhere, I basically didn't feel safe and something is up there with me. I am also aware that many of us feel this way, because we got caught in a feeling of loneliness. We felt a sense of unease. That is because everything is a process. Everything is a search. But also the importance</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>{'rand1': 46971, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 6218}</t>
+          <t>{'rand1': 78704, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 71396}</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDQ2OTcxLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDYyMTh9'</t>
+          <t>b'eydyYW5kMSc6IDc4NzA0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNzEzOTZ9'</t>
         </is>
       </c>
     </row>
@@ -2641,28 +2600,26 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Margaret asks the Wrong Question
-Performance notes: Few questions go to laughter faster than:
-©Photo: Hynek Maliksi, 2014, used with permission
-On mistakes, broken pens and fussiness
-I have a thing about things breaking. My wife keeps fussing with me about my pen never writing properly. When it's broken (and it happens nearly every day!), she explodes in fury, has "a temper tantrum", or does</t>
+          <t>2| Really? Charming, twerp?
+|2| Knowledge: It| (a) was a threat from God (ii) was a flashback from Beau Geste (b) was eerily dark - but if she knew an answer, she would have gotten them. So Michel de Bergerac left and proposes |
+= | --something in| (ii) is wrong, right?
+&lt;&lt;answered|-&gt;| by-&gt;| Michel de Bergerac</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-The main reason is due to one common link in all of these different accents I guess and that's 'humor'. 
-Saying "I woz robbed!" chuckling in response, hopping in a car full of gravel and throwing rocks at someone with a "Go away" tic in our vowels... something that's perfectly natural for us having grown up saying (they don't do it in many other accents) and yet extremely strange to</t>
+          <t>1. You're not going to be 100% deaf to accent differences. 
+2. You're not going to mishear every major vital difference between your own accent and other major accents. So you're more likely to see a person as more appealing because of the perception that they are more amenable to you understanding them.</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>{'rand1': 65307, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 41524}</t>
+          <t>{'rand1': 18141, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 18331}</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDY1MzA3LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDQxNTI0fQ=='</t>
+          <t>b'eydyYW5kMSc6IDE4MTQxLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDE4MzMxfQ=='</t>
         </is>
       </c>
     </row>
@@ -2677,28 +2634,29 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1MEN (ptr velocities may seem exquisite, but theyâ€™re not exactly pretty) and use very clever algorithms to prevent debris from realigning while we fly.
-State: ------------------------- | |
-Where:
-What we say: 1MEN (one month eventually only right)
-What happens: -
-Results:
-State: ------------------------- | (</t>
+          <t>10 billion flecks 1cm in diameter and disposed of hundreds of millions of years ago.
+What the What?
+- GravityScifiGuy
+New Gravity City - Space City
+Alan Horn and Leslie Moonves Confirm New Gravity Film
+&gt;&gt; Watch Video
+(LOS ANGELES, CA – May 5, 2011</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>3 light-years really isn't that far. Our current generation of vehicles is rockets trimed down to a barely liveable size.</t>
+          <t xml:space="preserve">1. NASA doesnt want the best available booster to blow up their wildly expensive toys. 2. Boosters dont SMS 3.mph. pretty sure the ISS doesnt move 140mph on its a t x 2 pier. 
+People actually need to be worried about the objects that got into it. </t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>{'rand1': 31059, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 78961}</t>
+          <t>{'rand1': 70041, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 40139}</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDMxMDU5LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDc4OTYxfQ=='</t>
+          <t>b'eydyYW5kMSc6IDcwMDQxLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDQwMTM5fQ=='</t>
         </is>
       </c>
     </row>
@@ -2713,24 +2671,27 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>【SPOUSE FACTOR】According to the research, it has been found that the basic person vulnerable exchange person is the newlywed spouse, because after the marriage, the spouse's heart and romance will not be like the rest of the people. Due to similar need to meet each other's social experience and affection, life will be poor. Burdened with too many feelings, the person dares not confront communication old form body language, which leads to impersonality and</t>
+          <t>1. It's because you are not used to it.
+2. It's because spiciness reduces impulses in your brain, which would never arise if we ingested a substance on regular basis.
+3. It's because certain Emotion-Regulation Functions become activated when we get new sensations coming from the different Nutrition and Flavor.
+4. It's because your body is getting more time to focus on the muscle contractions i.e. the</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-[source]
-If my nose is stuffy when I leave the restaurant, I know that I didn't taste truly bad food. If I had visibly tasted it, I wouldn't have just sat there.</t>
+          <t>1. Make sure you wash right after eating the pyramid (spiciness) because you will also be smelling it (pyramid). 
+2. I think something about loads of amino acids builds up in your system  and hinders your sinus chamber from draining 
+3. During pregnancy your saliva glands still works some but I don't know what causes it, come to think about it I get this everytime I eat some mexican food I'm allergic</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>{'rand1': 70464, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 85501}</t>
+          <t>{'rand1': 80311, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 13290}</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDcwNDY0LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDg1NTAxfQ=='</t>
+          <t>b'eydyYW5kMSc6IDgwMzExLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDEzMjkwfQ=='</t>
         </is>
       </c>
     </row>
@@ -2745,33 +2706,29 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-In simpler words, figuring out why that mate was so orgasmic that night.</t>
+          <t>______________________
+To vote on answers, click on locked answers. Answers which are locked have score added and score dropped by rank-up events.
+Star: Locked Answer (1 point by rank up event) (To vote on locked questions click on locked answers)
+I think this is actually a dedicated question for Do girls reach orgasm if you don't orgasm first. I would rather have it in the Women/Men topic
+At the moment, an answer to this question doesn</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t xml:space="preserve">*****************
-HeartMagnet94 wrote:A Hippocratic oath is just a rule... nothing more.
-————————
-A man is not complete except with a brain to connect his penis. Rudyard Kipling, The White Man's Burden
-Post Reply
-4 posts • Page 1 of 1
-Post Reply
-4 posts • Page 1 of 1
-Who is online
-Users browsing this forum: No registered users and 3 guests
-</t>
+          <t>1: Dream? (see linked page 1&amp;2, eg as a person who had DID I was sure I had  addressed all aspects of that before)
+2: contraction of the pharynx near entry 
+3: ~ their brains.
+Nothing concrete or factual, but there are several physiological explanations. This is mostly a guess, but I best guess would be local frill initiation, either uterine or vaginal, or</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>{'rand1': 81243, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 6666}</t>
+          <t>{'rand1': 28830, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 24013}</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDgxMjQzLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjY2Nn0='</t>
+          <t>b'eydyYW5kMSc6IDI4ODMwLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDI0MDEzfQ=='</t>
         </is>
       </c>
     </row>
@@ -2786,23 +2743,26 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Modern humans have evolved to have narrow faces, maybe to focus light to the eyes better and see in lower light. However, populations that have been around for thousands of years (e.g., the Neanderthal) have broader taken to increase efficiency in that area of the eye. If you look at most societies in modern days (central and eastern countries, eg) you can see the concensus on how to shape the face based on your region and metro status.</t>
+          <t>Δ). The number of jaw joints is reduced only slightly if we take the length of the skull ~150 - 160 mm in its anteroposterior axis, so we shouldn't worry about any practical evolutionary issues related to this.
+So it is a testable prediction: When evaluating evolutionary hypotheses, we demand that predictions are testable. &lt;![if!supportLists]&gt;&lt;![endif]&gt;
+&lt;![if!supportLists]&gt;6.
+&lt;![</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>7 Answers
-Question: ||Question|&gt;|&lt;|| Answers: Murphy Boone, Betty Indian, Alica Cesar, Frankie Garcia, Jeff Haskins, Dr. Kay, and Hannah White. Murphy Boone: Correct How long have we been here? Alicia Cesar : still be drawn back to the world I use to live in, yet I still love what I do. My name is Betty Indian and I am a professional ballroom dancer. Frankie</t>
+          <t>We want to look at other genders. Also humans are social animals, our tendency is to look for members of the same sexual identity.
+However there is, I believe, a learned behavior that comes into touchness the matter of race: the assumption that toughness is something one can pass down genetically (corroborate this by considering how the creation of a "self-defense" white)</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>{'rand1': 62045, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 91863}</t>
+          <t>{'rand1': 49968, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 49729}</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDYyMDQ1LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogOTE4NjN9'</t>
+          <t>b'eydyYW5kMSc6IDQ5OTY4LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDQ5NzI5fQ=='</t>
         </is>
       </c>
     </row>
@@ -2817,24 +2777,27 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-The images in that painting are available everywhere - in daguerreotypes, lithographs and other less-transmitted forms. So you can even use the image from an 1859 print on your iphone (or even sell/reproduce on your iphone). 
-More complex art pieces however, because they are based on such a simple and obvious composition (strings for lasers</t>
+          <t>4
+|
+Answer details
+Each year XMAS production for the range of iPhoto, but also be good news for the equivalent of to BAD PHOTOGRAPHIONEWSAportfolio is even better to sell a trip to the range is less, VS all the goods to BAD PHOTOGRAPHIONEWS to go to the XMAS TOY BOX AD</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t xml:space="preserve"> intestines of the flounder, and you cast it at the fire, you shall take of the intestines but of the gut with the belly. And Moses said, "It is the blood thereof that makes it unclean. Then you shall burn the flesh over."</t>
+          <t>1. The image itself, meaning the original artwork.   
+2. Prior Art makes it illegal to reproduce the image commercially, which is defined as reselling the original. A truly nonprofit project would not have prior art against them, as they would not be selling the image in the first place.
+Source: I'm a librarian for a scholarly public library.</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>{'rand1': 11895, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 63379}</t>
+          <t>{'rand1': 29303, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 40436}</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDExODk1LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjMzNzl9'</t>
+          <t>b'eydyYW5kMSc6IDI5MzAzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDQwNDM2fQ=='</t>
         </is>
       </c>
     </row>
@@ -2849,31 +2812,24 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1) coaches like to show their athleticism: watching them coach a game-day is pretty exciting. Seeing them in the locker room is pretty exciting. They dress the part to get in the hype.
-2) they are responsible for past and present players, and they are part of their community.  They will likely be hired by another youth league or even parents looking for assistance coaching their own kids.
-3) not like "Coach calls it like he sees it"</t>
+          <t xml:space="preserve">1) They dress up just as much as other coaches, they don't have to do a full suit/white shirt;
+2) It is a final risk. I am absolutely sure more coaches than just Jim Harbaugh has had an outfit completely destroyed during the hectic and sometimes crazy atmosphere of a game. I saw some pictures of Vince Lombardi and he was a dude in suit even in the elbowing my super bowl victory and his feet caught on fire. </t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
           <t xml:space="preserve">
-        fans demand it
-&lt;|ELIF|&gt;mycart|&gt; Question: If Heinz tastes different orange, why do kids call the tomato ketchup?
-Answer: 
-        according to the Toast
-THE END OF INDEX 
-&lt;|ELIF|&gt;Berenard|&gt; Question: Why did Leonardo move to the village when he found Bruno on the bridge?
-Answer: He love Bruno (even the</t>
+   SECTION 2:   A. N889Q  B. A87D6 C. O98Q6  D. R8QK6  Question:substring (stay) of substring (fly) lies: Stock#1 Stock# 2 Applying permutation (X|Y) = (X [Y]) [R]S36Q57 YL96F3X S356QU8L</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>{'rand1': 67546, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 64279}</t>
+          <t>{'rand1': 41990, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 76104}</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDY3NTQ2LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjQyNzl9'</t>
+          <t>b'eydyYW5kMSc6IDQxOTkwLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNzYxMDR9'</t>
         </is>
       </c>
     </row>
@@ -2888,18 +2844,26 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1) Single cell organism caused by H. Tiefenbach (many species, including the epitonin gene from Dictyostelium discoideum) is the first single cell oxygen producing creature that has significantly contributed to K+ stealing from blood. 2)Using tracing methods, wiggins and Sakalics showed this glucose can turn CO2 into oxygen and we know wiggins and likewise Jeffery were form</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr"/>
+          <t>0/10
+Obsignations: Trees are very important for the environment: All living creatures depend on trees. During the winter, the trees, plants, and other living organisms “hibernate” and gradually and regularly convert carbon dioxide into oxygen by plants roots and through photosynthesis. Plants produce oxygen by converting carbon dioxide into carbohydrates.
+It comes from: 4/8 lasts 13 days | 7 years (</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+http://www.youtube.com/watch?v=kJG06PfHRQs&amp;amp;feature=youtu.be
+trees are really **good** at photosynthesis. They take carbon dioxide over time and incubate in orange vests to fuel themselves for the winter. when you pass by, they turn all that chemical carbon into oxygen. it don't really get</t>
+        </is>
+      </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>{'rand1': 32267, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 56360}</t>
+          <t>{'rand1': 38026, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 64679}</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDMyMjY3LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDU2MzYwfQ=='</t>
+          <t>b'eydyYW5kMSc6IDM4MDI2LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY0Njc5fQ=='</t>
         </is>
       </c>
     </row>
@@ -2914,29 +2878,25 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t xml:space="preserve"> like to actually call it a genocide
-https://forums.straordinario.com/META1988-subject_H104.asp
-They went through a lot, but the deaths were estimated to be about 1/3 of all casualities during WW1 
-They probably say genocide because it's a word that carries alot of weight but there's hardly any proof the </t>
+          <t xml:space="preserve">
+The international etiquette of genocide recognition is less strict than most people expect. Genocides need happy endings, and they can't very well be 30+ years behind when it comes to recognition. 
+Historically, Turkey has taken the line that many problems in their relationships with the Armenians are simply a bad reflection on previous leaders, not their responsibility to acknowledge, and that serious discussion of this issue</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1945
-Slobo | 27.05.2017. | Original
-Why did people downvote a post with an existential threat to our democracy and the best denouncing of an injustice in history known as the genocide by the Turks?
-MILOIS | 25.05.2017. | Original
-Does Ireland need an opposition party that is obsessed with heritage and</t>
+          <t>1) For a FREE and Independent Armenia in a region being continuously occupied by Turkey and its Main Street client (Georgia), as Turkey literally empties its $$$ reserve in Georgia
+2) Not even gassing their own citizens in their sleep STILL, wouldn't compel Armenians to accept Soviet Armenians and Folks Almost Identically Like You! ([a href="#Benito" name="Benito"]See my Answer</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>{'rand1': 73997, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 2381}</t>
+          <t>{'rand1': 51797, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 85527}</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDczOTk3LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMjM4MX0='</t>
+          <t>b'eydyYW5kMSc6IDUxNzk3LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogODU1Mjd9'</t>
         </is>
       </c>
     </row>
@@ -2951,24 +2911,29 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-You can drink in any moving transportation. Trapani Argentina had to limit drink to essentuially no alcohol. Essentially buford prison had a great drinking gantlet to try to tip the scales
-Of course car is not traveling any control were stretchers or tools will be used so note it is still still smashing into your head at decent speeds so best practice is to leave it unless you cant drink on your feet then just not climb in</t>
+          <t>1. You are more secure as a passenger. Limousines are designed to protect you against theft, such that there is no easy place to place a drink to hide it from potential thieves. 
+2. There are laws in many states which forbid alcohol being consumed by the driver or passengers until they pass a road side sobriety test. Limousines are designed to not disturb other passengers on it's interior, therefore making it difficult for law enforcement to see</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>19 | &lt;&lt;&lt; Description | Eat Weigh: Starting Foods | &gt;&gt; ]]&gt; 2. Walnuts &lt;![CDATA[ Question: Two walnuts and a moose walked into a bar...[ Ref:] | &lt;&lt;&lt; Description | Wierd: Ya gotta luv it when the nuts fall out! | Start ay: Start your day off well... | Eat Weigh: Walnuts [ ] ]]&gt; 3. Sand! &lt;![CDATA[ Question: I</t>
+          <t>____________________________ __ ____ __ [BOOK]
+This question was taken from a different part of the book ____________ (see side notes for details).
+IDEAL QUESTION: Why did the bee eat the flower?
+IMPATIENT QUESTION: Is Cheesecake my mother's boyfriend?
+} "You want to know why my cave broke all the lamp?"
+| "God said, 'Ease my fucking way'?"
+Submitted</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>{'rand1': 20100, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 28439}</t>
+          <t>{'rand1': 24492, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 27539}</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDIwMTAwLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMjg0Mzl9'</t>
+          <t>b'eydyYW5kMSc6IDI0NDkyLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMjc1Mzl9'</t>
         </is>
       </c>
     </row>
@@ -2983,30 +2948,25 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>1) Superglue dries faster than water.
-2) I believe the answer is that superglue molecules are smaller, and capillary action is slower.
-3) Superglue dries fast enough that it ends up below the water level, and pulling up an old tube is more of a pain in the tush.
-Sorry for the mix of minute details. But these are two reasons that the product does not adhere to most other body parts or surfaces. And</t>
+          <t xml:space="preserve">
+Super glue has a low surface energy, which makes it hard to stick to itself.  The surface tension of the glue causes the thickened layer that forms on the top of the surface layer of the glue to repel each other.  After it has been in the bottle for awhile, the surface becomes progressively bumpier, and the same thing happens to that layer, resulting in the repulsion to produce more bumps. 
+It is the same reason why your finger won't stick</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1|&gt; &lt;|ELIF|&gt; The glue is in a bottle with a tight fit.
-Answer: 2|&gt; &lt;|ELIF|&gt; Remember that to stick to a glass surface, glue must have molecules that are small enough for gravity to pull to the bottom, where the surface is bigger. But super glue has not got such molecules. Thus it cannot stick.
-The importance of relations and relations of relations
-Summary
-|&gt; Answer: x&lt; y
-|&gt;</t>
+          <t>toys
+[LINK]-super-glue-with-game</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>{'rand1': 30713, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 93579}</t>
+          <t>{'rand1': 68200, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 58199}</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDMwNzEzLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogOTM1Nzl9'</t>
+          <t>b'eydyYW5kMSc6IDY4MjAwLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDU4MTk5fQ=='</t>
         </is>
       </c>
     </row>
@@ -3021,33 +2981,26 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1. you deposit a negative charge on silver oxide substances. ohms law will ensure that you pull excess + to ground.  
-2. Most Miners in the US are using batteries up around 95%-99.9% capacity for cheap. Hence your camera battery would probably have less than 1000 mAh capacity and less than 10% capacity.  
-Adding an unknown amount of silver, just a few cells in</t>
+          <t>_____________
+Merlined copy
+These pages cover “Non Sequiturs”, and the riddle in right-hand column is taken from Henry D. Ramm's Bizarro! of all the good writers (and illustrators) books I happened to stumble across over the weekend, Bizarro! served the purposes best as a collection of diablo clear basic explanatory stories, each focusing on a different reason a character, usually a Furry,</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1 :|
-I figure this is going to be the song of the thread soon:
-13 answers:
-9. Why do bathtubs float?
-8. Why is it called a sanitarium?
-7. Why is the enemy of my enemy my enemy?
-6. Who invented Go?
-5. Why are socks so expensive?
-4. Why does carbon monoxide smell like carrots?
-3. If you're speeding</t>
+          <t xml:space="preserve">
+Batteries were invented for being easily disposed of as a possible hazard to humans, so the batteries themselves don't actually need to be completely "usable" as they are too expensive to throw out.  
+When a battery is an obvious failure - like it simply refuses to do its job and doesn't even hold a tiny spark of charge - it has a higher resistance to the electrochemistry that is actually conducting the charge and therefore produces</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>{'rand1': 53818, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 83237}</t>
+          <t>{'rand1': 17291, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 7267}</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDUzODE4LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogODMyMzd9'</t>
+          <t>b'eydyYW5kMSc6IDE3MjkxLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDcyNjd9'</t>
         </is>
       </c>
     </row>
@@ -3062,22 +3015,28 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>236C Tobacco, Cigarette Smoking and Indoor Air Pollution. Epidemiologic Evidence of Tobacco Smoking and Air Pollution in the General Population: Testimony to the House Toxic Substances and Disease Committee. Testimony of to Brown, Frank, M.D. 1983 United States Department of Health and Human Services Testimony</t>
+          <t>0.9% of Questionable | o o lies.
+o o -
+no, they're too different
+o o the gays killing the innocense of americans
+o o Shot by HB on 2006-10-13 18:51 (Feb 06 2006) o |M|LIF
+oorly</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>&amp;gt; I may know what crack is, but I've never heard of amphetamine.</t>
+          <t>tobacco is not a drug, it's a plant, a weed.
+There is a different schedule in different countries.</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>{'rand1': 98856, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 86427}</t>
+          <t>{'rand1': 85891, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 3277}</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDk4ODU2LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDg2NDI3fQ=='</t>
+          <t>b'eydyYW5kMSc6IDg1ODkxLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDMyNzd9'</t>
         </is>
       </c>
     </row>
@@ -3092,34 +3051,24 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Opera Center
-one-pattern
-many-delete
-many-insert
-_________________________________________________________
-1:}
-LCCCBQ'WVAGEH (witness(L+canonize)
-returns:
-L CCC B Q' W V A G E H
-3:}
-LCCCWGIBRCDM (witness(</t>
+          <t>1. They are not integrated into western martial arts schools. 2. The Chinese martial arts tend to become more and more different as one goes back in time. Traditional Chinese martial arts has a lot of influences from the ever gloryed Mongol, Japanese and Korean martial arts. 3. Chinese martial arts lose what is the 'the art of wielding weapons'. Most of the Chinese martial</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>1. Chinese martial arts style don't get assimilated as Westerners expanded onto the East (ie: Karate would be recognised as Chinese, but it came from Okinawa &amp; Japanese); even its name is Chinese.
-2. Many Chinese military personal didn't want their techniques restricted by access to their practices, so they chose forms they could practice with complete anonymity</t>
+          <t>2 reasons (still miss a few though):
+1. Martial arts are cultural anachronisms. Tibetan cotton-monk kung fu has no older origin. 
+2. Historical anachronism - they are not strictly practical. If you get attacked by, say, bandits and you don't have feathers on you, you can't fly,</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>{'rand1': 92183, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 94648}</t>
+          <t>{'rand1': 27008, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 54064}</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDkyMTgzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDk0NjQ4fQ=='</t>
+          <t>b'eydyYW5kMSc6IDI3MDA4LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDU0MDY0fQ=='</t>
         </is>
       </c>
     </row>
@@ -3134,28 +3083,26 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>3 different explanations :
-1) As :) notes says, the voice box hits a new vibrato phase when you have a cold, or are sick, or if you place your hand on it. 
-2) The vibrations are actually higher. 
-They will be closer to what "normal" frequencies sound like, than when you're cold. 
-3) You just can't hear it louder. 
-Your brain gets used to the crispness of your</t>
+          <t>After a night of sleeping, the ducts that carry sweat from your head to your base of your neck accumulate sweat that is transformed into lumps that cause it to sound like you've got something lodged in your ears. In the morning take a clean Q-tip and a little Vaseline, and push back the lumps, eventually you should be able to sleep fine.
+Q) |&gt;ANSWER|&gt; Question: Can you explain how a hedge hog moves?
+Answ</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>00:58 Question: I really tanked in my classser quarter exams. Is there any way to hack the clearing accounts? Class-clear, awards stating that you are hidden from everyone/or locker clear maybe?
-Answer: 01:03 Question: Hey Jim, love the podcasts :). A lot of the questions I've heard from the other AmazonBasics users and personal recommendations about various HP devices eg, Inspiron, Chromebook, EliteBook,</t>
+          <t>1- Because deep within the outer part of the tissues called vocal cords, blood vessels attach.
+2- The blood vessels are moving and the vocal cord tissue is starting to stretch and stretch will give that raspy feel. 
+But if your going to say my voice when I wake up vesiculosa sound like shit, then you got shit for a voice.</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>{'rand1': 22524, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 36751}</t>
+          <t>{'rand1': 60573, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 58133}</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDIyNTI0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMzY3NTF9'</t>
+          <t>b'eydyYW5kMSc6IDYwNTczLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDU4MTMzfQ=='</t>
         </is>
       </c>
     </row>
@@ -3170,25 +3117,26 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>41. Human equality can exist only when all human beings are treated as equals
-- signature | teacher: | class: jh | note (Options) | 41 | 21
-- question | gogie12341: | class: IIM | 41 | Nanayee Baba Yes :Sign :(*)
-- question | teacher: | class: jh | note (Options) | 41 | 36 (upto</t>
+          <t>10 Answers: The processes of taking bearings on anythingMore Example Question: «こんにちはウィグィンキ他、私は投誘カップ。»More Example Question: A girl has snowflake tattooed on her forehead but cannot remember where she got them. She asks: Which spring follows the summer?
+Answer: The spring chasing the spring under the springMore Example Question: Las agujas que están en el zapato cont</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t xml:space="preserve">&amp;gt; to make a baby think is translation.  That is, imagine if we could somehow take the sounds of another language and tune it to identify the differences at birth?  That would be the language that they think in, at least for a time.  But that's the basis of how people develop in languages, so it's more of a "why yes and magic do exist" than a "see actual thing."  </t>
+          <t xml:space="preserve">
+ Usually, they will slowly associate patterns in speech and vocalisation with speech sounds. This is fairly easy to learn.  Two of the most common are American/Cantonese/Japenese and mid-Eastern (Semitic).  
+Most serious languages (very complicated and varied) are either hopeless to learn "natively" or impossible, no matter how much effort you put into it.  
+edit: tonight voted hot</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>{'rand1': 11055, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 78809}</t>
+          <t>{'rand1': 37974, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 49590}</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDExMDU1LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDc4ODA5fQ=='</t>
+          <t>b'eydyYW5kMSc6IDM3OTc0LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDQ5NTkwfQ=='</t>
         </is>
       </c>
     </row>
@@ -3203,30 +3151,31 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 criteria-
-*They have hundreds of feet of HT Plastic on them.
-*They have very dense felty coverings over them.
-*They have extremely strong fiber structures that break down &amp; hold considerably. 
-</t>
+          <t>1 It's laminated glass, that's what I heard.  
+[LINK]
+  -  Source: graphite weilding it before the pins were introduce.
+Edit:  The above already answered the *why* question. How is the surface resistant to all of the nastiness?  How about utilizing it per complex lanes.  
+For those not already familar with the sport:  
+Lanes are</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>1 – Bowling ball tips have harder and harder plastic.
-2- Get a grip of the ball. My book says that grip is the most important factor before any other.
-3 – Allow the ball to adjust and "sweep" back on the lane when bowls pass it.
-4- The more weight you apply to the ball, the more extreme the upper ball is allowed to "sweep".
-5 – House that comes before bowling</t>
+          <t>1)We use special types of core or what we refer to as "bulls-eye core"(need explanation on this).
+2)Every current bowling ball is just stainless steel which kinda soft texture makes it less efficient for chopping down bowling pins.
+3)It is still a mystery as to why this isn't achieved by plastic?
+q
+Can you tell me why plates and irons were titanium in the kitchen during</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>{'rand1': 78150, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 54039}</t>
+          <t>{'rand1': 1697, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 87624}</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDc4MTUwLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNTQwMzl9'</t>
+          <t>b'eydyYW5kMSc6IDE2OTcsICdkb19zd2FwJzogVHJ1ZSwgJ2Fuc3dlcjEnOiAnM0JfY3AtMjUwMC5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAncmFuZDInOiA4NzYyNH0='</t>
         </is>
       </c>
     </row>
@@ -3241,27 +3190,26 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>took me awhile to find this:
-[LINK]</t>
+          <t>15-20 minute anuses.</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>〈EM|money|&gt;
-Question: Exactly where and how is the world going?
-Answer: Four[4] mystery quantities present on the lottery suit(suit)-number-pair(s) on the show...
-Question: Life Style~oTH~z is destroyed!
-Answer: あ(あああ)あ(あああ)あ(あああ)あ(あああ)あ(あああ)あ(あ</t>
+          <t>4 men selling "Quality Energy"太陽電 Fortune 话题 | 55 狗类 | 036
+鋸 | Phrasebook | goods | management | soft soft koss | works words | activate friendly | humm | cursor | affectionate modal | pick | touch | handle | sign
+Japanese-English Japanese-Chinese | N58
+[Today, 10:40] Shuu:
+[</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>{'rand1': 98177, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 8192}</t>
+          <t>{'rand1': 8662, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 43433}</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDk4MTc3LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogODE5Mn0='</t>
+          <t>b'eydyYW5kMSc6IDg2NjIsICdkb19zd2FwJzogVHJ1ZSwgJ2Fuc3dlcjEnOiAnM0JfY3AtMjUwMC5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAncmFuZDInOiA0MzQzM30='</t>
         </is>
       </c>
     </row>
@@ -3276,26 +3224,25 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>heres another thought: Why are they controversial because they 'keep kids from smoking', but not because they offer people who aren't allowed to smoke all of the chemicals audiences will be exposed to by smoking because they're uncomfortable with smoke?</t>
+          <t>100g of blubbery lungs
+1000g of cylinders
+3,000,000g of tobacco
+And in the end it just tastes right</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t xml:space="preserve">
- * 
- * Mist: The atomiser needs to be attached to a very fine metal tube, called an atomiser pipe or coillt. It is finished in a clear plastic casing 
- *                to look like a stick of cigarette but lit from the bottom, with a mixture of Quiter fluid and flavouring &amp; nicotine.
- * Vaping: basically what eCigs are all about, the way e-vap is controlled determines how damaging or non-dam</t>
+          <t>←|E-cigs|&gt;&gt; are the latest smoking cessation product that delivers what Nicotine Replacement Therapies (NRTs) like gum or patches can only dream of; Bowl spread: Nutella, strawberries on Low-Fat Rocky Road.</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>{'rand1': 73859, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 16413}</t>
+          <t>{'rand1': 2534, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 11365}</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDczODU5LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMTY0MTN9'</t>
+          <t>b'eydyYW5kMSc6IDI1MzQsICdkb19zd2FwJzogVHJ1ZSwgJ2Fuc3dlcjEnOiAnM0JfY3AtMjUwMC5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAncmFuZDInOiAxMTM2NX0='</t>
         </is>
       </c>
     </row>
@@ -3310,24 +3257,27 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>2000 years ago it was legal to do such a thing in Rome.
-But.. The Roman Empire collapsed because of it. Maybe it did that to its own citizens.</t>
+          <t xml:space="preserve">
+[LINK]-CARD/ Dungeons_and_dragons-HARMFUL-TO-MENTALLY_INFECTED-(based-on-facts).jpg
+With great power comes great responsibility.</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2 points. Source: Census. Social Concern. September 19, 2010. American Community Panel. http:// QUESTION: Are there any negative consequences to smoking pot, if not, why has it been illegal for so long? (2 points)&lt;/P&gt;
-&lt;P&gt;Answer: 2 points. Source: Census. Social Concern. September 19, 2010. American Community Panel. http</t>
+          <t>1) If people assume that marijuana is more harmful than alcohol, our support is limited. 2)...
+1 page
+“I don’t Like To Lose” : An Analysis Of 8 Strategies To Orient Moral Support By The Child, Team Or By The Adult Who Is Caregiver An, Raising Children, Personal Values, Concepts And Principles
+A long time ago Earl Holley’s family decide on beginning a university education because</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>{'rand1': 76813, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 52069}</t>
+          <t>{'rand1': 43664, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 49769}</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDc2ODEzLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNTIwNjl9'</t>
+          <t>b'eydyYW5kMSc6IDQzNjY0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDk3Njl9'</t>
         </is>
       </c>
     </row>
@@ -3342,23 +3292,29 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>1% decrease is probably more than what you mean.  There's also some slow hair loss as well as genetic predispositions, you may need medical attention.  
-A good part of the answer is that hormones that stimulate hair growth happen to start decreasing in men around the same time that being less hairy seems to start decreasing: puberty and adolesc</t>
+          <t>......................
+QUESTIONS PREVIOUSLY ANSWERED:
+• What's the distihtuion between Cystic Fibrosis and Beta-glucourbideuria?
+• What's the difference between Coproporphyria cutanea tarda and Alcoholic Dermatosis?
+• Wht are b</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>1. Testosterone levels ear ly climb e and h igh S up or c h ild rearing. 2. Testosterone levels f aller waxing and g your se in tern. I sta ilit y or smoothly and never shave. 6. Testosterone levels u tilde men are da yd of ih itations. 7.</t>
+          <t xml:space="preserve">
+Yes but the top layer is shed.
+Basically you have a bunch of peach fuzz which eventually peels off. 
+The reason we do not notice the second layers is their color is black, which interferes with light processing.</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>{'rand1': 9354, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 28888}</t>
+          <t>{'rand1': 8326, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 81207}</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDkzNTQsICdkb19zd2FwJzogVHJ1ZSwgJ2Fuc3dlcjEnOiAnM0JfY3AtMjUwMC5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAncmFuZDInOiAyODg4OH0='</t>
+          <t>b'eydyYW5kMSc6IDgzMjYsICdkb19zd2FwJzogRmFsc2UsICdhbnN3ZXIxJzogJzNCX2Jhc2VsaW5lLmFuc3dlcicsICdhbnN3ZXIyJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ3JhbmQyJzogODEyMDd9'</t>
         </is>
       </c>
     </row>
@@ -3373,25 +3329,25 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>6. What does Carnegie Mellon University do as a high school student?
-What is Your Ultimate T-shirt?
- wasn't Australian: the people wore the costume, they did not CHANGE their own basic body characteristics to become princesses...
-Quality X-Ray Glasses
-Product specifications -- From HighBeam Research.
-Why Did It Beln Hell
-Why did it burn? For why touch is prohibited?
-YAMANT</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr"/>
+          <t>2 alpha strands (helix dimers) and 1 y-strand protein (2 chains + 1 y-strand) form an alpha helix formed by 3 DNA-molecules, bound together into a very stable compact structure (thus a DNA-guide). That's why DNA-guide (alpha helix) guides your body in getting fit.
+Disease, forgetting or wasting your DNA in you're body</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2 million years ago kind of problem solving in a harsh environment would have meant survival of the 
+strongest.
+in fact edit: polluted water doesn't kill you as quickly, it does cause a huge PH change in the body.  Excrement is acid and the change in the PH creates a lot of respiratory issues.</t>
+        </is>
+      </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>{'rand1': 29611, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 65362}</t>
+          <t>{'rand1': 96496, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 90553}</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDI5NjExLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY1MzYyfQ=='</t>
+          <t>b'eydyYW5kMSc6IDk2NDk2LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDkwNTUzfQ=='</t>
         </is>
       </c>
     </row>
@@ -3407,27 +3363,24 @@
       <c r="C87" t="inlineStr">
         <is>
           <t xml:space="preserve">
-AppleScript and Apple Events point out the Extent field in the CD_DiskInfo dictionary. 
-Using this field we can determine when the audio stops.
-If you do FileMaker what about incorporating the AppleScript code above. 
-Otherwise just listen for Quit:... after each action you want to take care of.
-</t>
+[LINK]-Englisch/watch/- footage_22202969_900.html</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>1) the device has a sumbitted error, means it must do something to alert in case of a problem (let's say it's music, play until its dead silence, not sure what the norm is here)
-2) in case no one survived, the media (the little bits like music etc) are still there and there is a backup (hopefully)</t>
+          <t>26 May 2003|&gt;Infinite|&gt;Dolphin endearing to Dolphin Before reaching the Dolphin itRandom|&gt;Options: Page Last Modified: 10 Sep 2008|&gt;Numbers or Words|&gt;Translations|&gt;On a Stack Snippet Base Path you are trying too |&gt;Jabber User
+Does a mill make a saw?
+Yes, in the literal sense. When you rotate a piece of wood,</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>{'rand1': 29423, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 89260}</t>
+          <t>{'rand1': 43523, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 93589}</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDI5NDIzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDg5MjYwfQ=='</t>
+          <t>b'eydyYW5kMSc6IDQzNTIzLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogOTM1ODl9'</t>
         </is>
       </c>
     </row>
@@ -3442,25 +3395,23 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>1st we need mass, 2nd we need complexity, the reason we name them "chemical weapons" is
-1) their origins, 2) they're blatantly poisonous. (why poison the leader of your enemy in the worst possible way....whats the next step?) And are used in warfare of nasty ways in the worlds now!
-(there are herbal colon cleansers... that don't</t>
+          <t>10 years old here  
+why?</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1) Special weapons have another name they use depending on the nature of the weapons.
-2) Yes.  Most materials are classified as weapons, chemically.</t>
+          <t>1st, one can't make something killing out of nothing. 2nd, some Russian officials said the Russians would respond with tactical nuclear weapons if necessary. But since all the WWIII bombs only cover a distance of 100 kilometers and not too much ones, the President is making precautions to deal effect. Using fewer atomic bombs is better since it doesn' No.1 weapon (sometimes called as Socrates "</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>{'rand1': 33989, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 68791}</t>
+          <t>{'rand1': 89521, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 13265}</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDMzOTg5LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY4NzkxfQ=='</t>
+          <t>b'eydyYW5kMSc6IDg5NTIxLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMTMyNjV9'</t>
         </is>
       </c>
     </row>
@@ -3475,23 +3426,23 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>10 million macrobols (one half will go through starvation)
-Eminem Ate One HALF-sized pizza after his meal today.</t>
+          <t xml:space="preserve">2000 calories is not "enough", it's just maybe a little less than you need. That's why some stuff like restaurants don't say you should eat like 2000 calories to sustain your average daily habits. </t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2000 calories worth of food in one sitting should give you enough energy to keep you going, provided you're actually taking in those calories</t>
+          <t>1, 100.
+Pythagorean theorem: \(\sqrt{a + b} = \sqrt{ab} \) Question: What is the value of \(\sqrt{abc}? \) Explain why x^2 - 2x + 4 = 0 is an example of a quadratic function whose graph has two sets</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>{'rand1': 79635, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 83459}</t>
+          <t>{'rand1': 20544, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 74129}</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDc5NjM1LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDgzNDU5fQ=='</t>
+          <t>b'eydyYW5kMSc6IDIwNTQ0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNzQxMjl9'</t>
         </is>
       </c>
     </row>
@@ -3506,27 +3457,23 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>10, so its cheating.</t>
+          <t>75%+ of added cleaning chemicals are removed by another process after filtering.
+Furthermore,  dignity.</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t xml:space="preserve">58% Yes. 42% no="" /&gt;
-50th Anniversary of the Nuclear Accident, Number Two in the Series
-Author: Michael Fairman. On a much larger scale Chernobyl, more specifically power station No
-2 at Chernobyl, was far more damaging to the environment.
-Chernobyl
-Chernobyl, Ukraine; 13 April </t>
+          <t>1) That depends on a fairly simple chemical reaction of precipitation. If these additives dissolve in the water, then a large amount of minerals and serve as a source of fluoride in the water when it is practiced by hand in a home nearly always. with 2 or higher fluoride content at a time, which are known to vary in basis is not an accurate scale. Most urban water is</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>{'rand1': 21210, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 62685}</t>
+          <t>{'rand1': 43115, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 64379}</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDIxMjEwLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjI2ODV9'</t>
+          <t>b'eydyYW5kMSc6IDQzMTE1LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjQzNzl9'</t>
         </is>
       </c>
     </row>
@@ -3541,26 +3488,24 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>► The change in shape is exaggerated, because doing so increases the surface area.
-In addition, the presence of hydrogen ions releases pressure and makes the ice fragile
-However, hydrogen is not know production, its existence is defined in the living breathing enzymes of biological systems
-It is fluid, renewable and constant. Like our breathing. We have a constant challenge to supply us with erinaceus ( hydrogen). Know for dead killed pigs as pork</t>
+          <t>1. When cold things contract and warm things expand, cold obeys Heat Death Right, while warm things obey Heat Death Left. This means the heat being supplied by the Sun in this case is uniform throughout the object and hence equal to the total temperature of that object. Further, we know that volume x temperature is constant, which assures volume and temperature to remain constant.
+2. When cold things contract, warm things expand, temperatures of both sides remain</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Water does expand when it changes from a liquid to a solid. The cold gets colder so it gets denser while the warm gets warmer so it gets fewer molecules per cubic meter. </t>
+          <t>1. When warm things expand, their molecules are rubbing against each other. At lower T they are sliding down the walls with a lot more energy. This causes more force. So ice is kind of a strange state of matter.
+2. Also, you're forgetting the surface tension of water (and other liquids). When you cool something to freezing, that surface area gets smaller. So you have to put more molecules on there to cover</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>{'rand1': 13287, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 91630}</t>
+          <t>{'rand1': 57971, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 12696}</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDEzMjg3LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDkxNjMwfQ=='</t>
+          <t>b'eydyYW5kMSc6IDU3OTcxLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDEyNjk2fQ=='</t>
         </is>
       </c>
     </row>
@@ -3575,22 +3520,23 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>3.5 GHz i5s of Intel Core are designed for laptops powered in 13.3'' or 14'', but an i7 processor of Intel Xeon or Core can not be fitted on a laptop without 3rd part heating elements. Because of that I would not buy an i7 in laptops with i5 processors. The bottom line is it is irritating that laptops with i7 processor are still</t>
+          <t>3.5Ghz comes on an i5. if you bought a i7 it might be 4.0 or 4.5Ghz. i7 usually has an at a higher clock speed but requires a higher power supply for the extra heat it produces.
+these aren't even the same processor. the Phenom II has a 3.6 GHz version. just making sure that points out how</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>10% performance between these 2. Thats it.</t>
+          <t>3.5 GHz; 2.6GHz</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>{'rand1': 15453, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 5863}</t>
+          <t>{'rand1': 40893, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 15522}</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDE1NDUzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDU4NjN9'</t>
+          <t>b'eydyYW5kMSc6IDQwODkzLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMTU1MjJ9'</t>
         </is>
       </c>
     </row>
@@ -3605,27 +3551,20 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>6 weeks in the fridge (sometimes it's kept for longer) causes them to become overly sweet and is what makes them likable.
-This is the result of glucose becoming more concentrated due to being exposed to a different chemical environment.</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-*
-*The shelf life of prepackaged cookies is one year, whereas the shelf life of prepackaged cookies is one year.
-*They are made up of batches of thousand of cakes on a large scale to match the production time.
-*These pre packaged</t>
-        </is>
-      </c>
+          <t>1000 layers.
+Of the above answer, Cal NS explains:
+I believe your logic is flawed (at least for most cookies). While there are the important variables of flavor, e..g. chocolate chip cookies vs. chocolate crinkle cookies, those are affected equally by manufacturing.</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr">
         <is>
-          <t>{'rand1': 25764, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 22396}</t>
+          <t>{'rand1': 96713, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 28728}</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDI1NzY0LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMjIzOTZ9'</t>
+          <t>b'eydyYW5kMSc6IDk2NzEzLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDI4NzI4fQ=='</t>
         </is>
       </c>
     </row>
@@ -3641,26 +3580,26 @@
       <c r="C94" t="inlineStr">
         <is>
           <t xml:space="preserve">
-#### What newcomers should know 
-It is part of the Circadian rhythm.  After the body's clock hits the sleep or light "mood" period it thinks it needs to eat to reset and redevelop the sleep/casual and so on cycle
-So eating at that time, particularly to the point of excess can overload the system, and so the body thinks is in a "danger" period and fatty acids called Adipose are</t>
+Well basically, your body is expecting food to be around all day. In the morning, the sun makes you wake up and feel hungry because it's light, making it seem mid-day even if it's night.
+Also, it's hard to avoid having carbs in the morning because it's a trap to start your body off right. If you never ready after the night, you're most likely to feel hungry.</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>ummmm, don't wanna cause any alarm here but thats because tootsie rolls are the best reaction to that question i could ever need foo....
-Question: My cousin is really making me depressed by calling me more than two times a day even though she had already told me that she was busy the next day?
-Answer: To be honest with you, that's actually pretty normal. Teenagers obviously have a lot of stuff on their mind all the</t>
+          <t>15 seconds later you'll be ready to explode, because you'll have consumed everything that willd leave your body in the next period.
+Know your seconds…in a Tic-Tac-Toe game,hours you've won at 300 dollars.
+ThinkstockPhotos.com
+A) 1..5..9..13..17..23..31..GET A CLUE</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>{'rand1': 29920, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 61083}</t>
+          <t>{'rand1': 89697, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 69707}</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDI5OTIwLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjEwODN9'</t>
+          <t>b'eydyYW5kMSc6IDg5Njk3LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNjk3MDd9'</t>
         </is>
       </c>
     </row>
@@ -3675,28 +3614,27 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>5|HOW_AFRICA_99 |___Math%11|ELIF|_Line%11|&gt; &lt;|MY|&gt; &lt;|
-47
-The Nude Male Drowning Scene
-” The laces were hidden in the dead man’s pocket, and they took it from his pocket” He initially imagined that the dead male was drinking too much and drown himself in the sea “The policeman said eventually and as the policeman was</t>
+          <t>__________
+| Pam|GUY|Logic|Joe| build a house of cards, and if you hit one blow you have
+|JOE|(Solve some equations)|Pam|(Solve some equations)|stamped the cookie adventurous surviving the more so be a of
+|Jubba|Logic|Joo|dick|dick|dick|Initials
+|Pam|TECHNIC|Backgroud|Jamb|Management|</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-* After increasing doses the user would go into convulsions due to the excess stimulation of the brain and body's reaction to the drug that is missing..
-* Because the brain loves and looks for stimuli the final overdose of stimuli would cause pretty rapid death.
-* OR the person without a stimulant may become quite euphoric itself on the absence of stimulant which will cause fatal heart failure.</t>
+          <t>1. Diversion.  If the drug took precedence over everything else in their life, maybe if the authorities tried to make them leave for a more addictive drug, they would fight back so hard they would put themselves in prison until they got the help they needed.
+2. Predisposition.  According to a study published this month, past use of drugs might make you more likely to get addicted to the next one.  Alcoholics have</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>{'rand1': 28421, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 80240}</t>
+          <t>{'rand1': 25231, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 40458}</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDI4NDIxLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDgwMjQwfQ=='</t>
+          <t>b'eydyYW5kMSc6IDI1MjMxLCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDQwNDU4fQ=='</t>
         </is>
       </c>
     </row>
@@ -3711,27 +3649,35 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>12 bones
-2. To bend your knee as far as you can, hold one leg with your hand, pull the other to you and let go of both legs. Repeat. Name ______.
-3. Explain where your elbows come from
-4. If your elbow is normal, Superman won't fly, the cat won't pounce, and we must not worry about a backboarding/shot block protectors.
-5. Your elbow joint (humer</t>
+          <t>3!: 13
+Wordplay Difficulty: Time Limit: -150ms
+0.241sec
+75
+Flag
+0
+Flagged by:
+ CambriLao
+4 Answered Questions
+[–] SpartYan 0 points last 30 days 0 points all-time
+-2
+[+] FADD attempts to improve the feature explaination Dude speaks raytracing to me
+-9</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>1 million years of evolution resulting in specialized body/limbs makes happens. You're born with the number of different joints in your body that you have. The hands is one, the feet are another, the back is another, the jaw another etc. If your joint is a bit more flexible than average then you'll be able to do stuff you may not have always been able to do before.
-edit: modified tldr</t>
+          <t>Ask that guy whose legs and arms are completely able to do everything a double joint person's arms and legs can do.  They often can play any sort of sporting event (tennis to baseball etc.) without problems.
+Although many double joint people have severe scoliosis, there are those who are able to have a normal Jellyfish like spine, allowing them to walk upright with only mild scoliosis(although many have many chairs!).</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>{'rand1': 424, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 12885}</t>
+          <t>{'rand1': 2781, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 12605}</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDQyNCwgJ2RvX3N3YXAnOiBGYWxzZSwgJ2Fuc3dlcjEnOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfY3AtMjUwMC5hbnN3ZXInLCAncmFuZDInOiAxMjg4NX0='</t>
+          <t>b'eydyYW5kMSc6IDI3ODEsICdkb19zd2FwJzogRmFsc2UsICdhbnN3ZXIxJzogJzNCX2Jhc2VsaW5lLmFuc3dlcicsICdhbnN3ZXIyJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ3JhbmQyJzogMTI2MDV9'</t>
         </is>
       </c>
     </row>
@@ -3746,25 +3692,28 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t xml:space="preserve"> no, im glad someone asked about this kind of shit, ive seen it my life time, they just laugh for no reason whatsoever at what ever they see, or because it just seems funny to them, whether its a serious video or just an old man, trying to get their taxes done, im pretty sure theyre just really shut off mentally. 
-they laugh in front of people, and appear seemingly phased with everything they do, constantly moving around feel a little sticky</t>
+          <t xml:space="preserve">
+“Say a word with an [  ]( http://www.mime-life.com/mimopictures/Mimopics/29msm018.gif  ) sound to them. They're even funnier than usual.
+Give them a loud, difficult laugh. They even crack up more than usual!"
+I know I am a throat-clearing, fore-chewing sobs who laughs,</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>100% YES
-What did I have in mind when I wrote this? Well, in the days that I was boarding in a boarding house in Kista, Did you know that Mads Mikkelsen, the hitman from the popular Danish/German TV-Hit ganzerstrasse who has made a name for himself in hit-man and other series and movies is a friendly person? Well, that is what I have :0)
-Funny pages</t>
+          <t>umm... yeah...
+Date / Time Monroe receiving, Zed research in progress
+Duration 3:37
+Reference Apr 28, 2017 / 09:28...</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>{'rand1': 50175, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 20276}</t>
+          <t>{'rand1': 30758, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 48179}</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDUwMTc1LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMjAyNzZ9'</t>
+          <t>b'eydyYW5kMSc6IDMwNzU4LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogNDgxNzl9'</t>
         </is>
       </c>
     </row>
@@ -3779,23 +3728,29 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>1) Other companies are selling for about $2.10 tickets (Kayak.com) when leaving a $2.50 would make these tickets a bit further profit.
-2) Monopsonistic world</t>
+          <t>1) Stamp
+2) Postage
+3) Paper
+4) Paper
+5) Mail box
+6) Effort by the postal worker and the post office to tigger the printer-people hate that
+Who decides how much is being charged to mail stuff?  Can the customer demand the further charge to be removed?  Who knows what they're not being told?
+Umm</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2.50 to print your ticket does NOT mean that the coupon is actually paying for ANYTHING. Almost every ticketing transaction you have had in the past (even the FREE ones) have made some sort of payment to the venue and/or box office. The problem with our current system is that $2.60 was paid and the $2.50 is just gravy. The 10%</t>
+          <t>1. Ticketmaster does not charge a fee to print tickets if they are pre-purchased on their site, and any other charge is because of the printer used to print tickets. Ticketmaster does not choose which printers to trust, but rather allows any number of printers to bid for a printing job. If the printer who wants the job, does not have the correct ink or toner or does not meet any of the</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>{'rand1': 92162, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 3375}</t>
+          <t>{'rand1': 72267, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 28127}</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDkyMTYyLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMzM3NX0='</t>
+          <t>b'eydyYW5kMSc6IDcyMjY3LCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMjgxMjd9'</t>
         </is>
       </c>
     </row>
@@ -3810,25 +3765,33 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>0&lt;|ELIF|&gt; A real pussy will turn into a pussycat.
-preamble, character and code are all different... and sometimes missing :-)
-help us with this summation I'll donate 1 Euro for every 5 lines found
-Page created in 0.136 seconds with 74 queries.</t>
+          <t>5 years
+4. |4| Question: what makes a living being non living?
+Answer: 6 years
+5. |5| Question: What is non living
+Answer:
+self
+6. |6| Question: Dogs and cats are non-living. Non of them are alive. explain
+Answer: 4 year span, students should break into groups and solve "playing ducks" one experiment at a time
+Students also work in their groups</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 weeks is enough time for bacteria and other things to build up that would make you sick. If you ate that food chance are very high you would get sick and die. </t>
+          <t>1) inside is oxygen and decompose stuff.
+2) body can use it better, for it's own growth. 
+edit: good one isubi.
+edit 2: wrong word. saying that the dead body is dead because it not living anymore, but the skin does not function anymore, like skin does not dry, if your body is dead.</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>{'rand1': 82948, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 17895}</t>
+          <t>{'rand1': 16467, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 51141}</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDgyOTQ4LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDE3ODk1fQ=='</t>
+          <t>b'eydyYW5kMSc6IDE2NDY3LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDUxMTQxfQ=='</t>
         </is>
       </c>
     </row>
@@ -3843,25 +3806,27 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>1) It is packed with carbohydrates 2) glucose is known as a primary truck in ketosis, blocking ketone acetone from doing its job. Make sure your dog is ingesting food that not have carbs in it.
-26:43 | 1 year ago
-Patient dies of sepsis despite ‘miracle’ intervention |9∈⋯∪:20.92 in 2021</t>
+          <t>3/27/2007 = 0220 | 03/27/2007
+The “date calculated” has to do with the program and the “date entered” of the person logged in now. The programs can be running now with the date being entered or someone else who came in today and their date is used for the date entered. It won’t matter that it may be 5500 miles or a</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>1. She has a stomach, not a head, and she doesn't actually eat food. She only barks/jumps/etc.
-2. Dogs are pack animals. It's how they survive. Over time, aftergassing, their tongue becomes oilier, tasting less it of the faint taste of cooked animal matter. Once stung with portion, either from purely accidental expulsion, hungrily in balance</t>
+          <t xml:space="preserve">1 part of it is their natural pack dynamics- they won't eat what those around them eat and you will too in an attempt to early nest.
+It's also conditioning through their mother. She will teach them to:
+1) stay away from non-mammals (people food) to me her and prevent anyyself from becoming "sick"
+2) avoid harping human scent
+</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>{'rand1': 88655, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 42194}</t>
+          <t>{'rand1': 23897, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 69599}</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDg4NjU1LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDQyMTk0fQ=='</t>
+          <t>b'eydyYW5kMSc6IDIzODk3LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDY5NTk5fQ=='</t>
         </is>
       </c>
     </row>
@@ -3876,32 +3841,28 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t xml:space="preserve"> the epidermal layer of Atlantic salmon is shiny, giving them a unique coating that discourages them from getting parasites.  Salmon from the elsewhere don't have this, so they have to become parasite-free first before they can be sold to people.  
-The shinyness is not the only factor that contributes to avoiding parasites.  
-P答erator</t>
+          <t xml:space="preserve">
+&lt;|Answer|.&gt;|&gt; A: Because of the rich food chain in the Atlantic. See, the Pacific is where us humans live on top of the ocean 
+The peasant grows chickens on the Pacific salt water (since they’re salt water fish), so the water is rich in large animals (which provides a larger, richer, 
+Answer 
+Ask me for a polymath, and I’ll hang you upside down</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>145
-63.
-Food Worldwide Question: What foods traveled overseas the longest?
-Answer: 159
-Illegal Here Question: What food did Washington D.C. outlaw in 1976?
-Answer: 63
-Food Telecourse Question: What was first served in colleges and became a preferred dish for students?
-Answer: 39
-Breakfast Food Question: What common breakfast</t>
+          <t>1. Washington is a huge state in the Pacific, so they have more natural treatment of salmon where the Atlantic generally only sees people
+2. Wild salmon from Washington are smoked and brined/salted to remove parasites
+3. They're quite tasty despite being parasite-heavy</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>{'rand1': 66573, 'do_swap': True, 'answer1': '3B_cp-2500.answer', 'answer2': '3B_baseline.answer', 'rand2': 2169}</t>
+          <t>{'rand1': 44917, 'do_swap': False, 'answer1': '3B_baseline.answer', 'answer2': '3B_cp-2500.answer', 'rand2': 36298}</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>b'eydyYW5kMSc6IDY2NTczLCAnZG9fc3dhcCc6IFRydWUsICdhbnN3ZXIxJzogJzNCX2NwLTI1MDAuYW5zd2VyJywgJ2Fuc3dlcjInOiAnM0JfYmFzZWxpbmUuYW5zd2VyJywgJ3JhbmQyJzogMjE2OX0='</t>
+          <t>b'eydyYW5kMSc6IDQ0OTE3LCAnZG9fc3dhcCc6IEZhbHNlLCAnYW5zd2VyMSc6ICczQl9iYXNlbGluZS5hbnN3ZXInLCAnYW5zd2VyMic6ICczQl9jcC0yNTAwLmFuc3dlcicsICdyYW5kMic6IDM2Mjk4fQ=='</t>
         </is>
       </c>
     </row>

</xml_diff>